<commit_message>
modificaciones en los bosquejos de las interfaces de los dos registros y actualizacion de la informacion de la base de datos
</commit_message>
<xml_diff>
--- a/trabajos-of-publicaciones-e-impresiones-uncp.xlsx
+++ b/trabajos-of-publicaciones-e-impresiones-uncp.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4300" uniqueCount="2257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4355" uniqueCount="2287">
   <si>
     <t>Documento</t>
   </si>
@@ -6774,9 +6774,6 @@
     <t>oficina de bienes patrimoniales - facultad de ciencias agrarias de satipo</t>
   </si>
   <si>
-    <t>oficio n° 0475-2011-BP-BRAC-UNCP</t>
-  </si>
-  <si>
     <t>vicepresidente académico de la comision de orden y gestión</t>
   </si>
   <si>
@@ -6787,6 +6784,99 @@
   </si>
   <si>
     <t>al 153,438</t>
+  </si>
+  <si>
+    <t>oficio n° 0475-2011-BP-VRAC-UNCP</t>
+  </si>
+  <si>
+    <t>oficio 115-2011-J-OGCAL/UNCP</t>
+  </si>
+  <si>
+    <t>oficio 325-2011-DFEN-UNCP</t>
+  </si>
+  <si>
+    <t>oficio n° 0409-2011-SG</t>
+  </si>
+  <si>
+    <t>oficio 132-2011-OGCAL/UNCP</t>
+  </si>
+  <si>
+    <t>oficio 159-2011-CEE-ANR/UNCP</t>
+  </si>
+  <si>
+    <t>Victoria Salcedo Matos</t>
+  </si>
+  <si>
+    <t>Comité electoral externo ANR</t>
+  </si>
+  <si>
+    <t>Impresión de 6 fotografías</t>
+  </si>
+  <si>
+    <t>Apoyo con el diseño de afiche</t>
+  </si>
+  <si>
+    <t>Apoyo impresión de certificados de convenio</t>
+  </si>
+  <si>
+    <t>Confección de libros de grado de bachiller y titulos profesionales</t>
+  </si>
+  <si>
+    <t>Impresión de 200 afiches sobre acreditación</t>
+  </si>
+  <si>
+    <t>Diseño e impresión cédulas votación estudiantes representantes ante asamblea universitaria, consejo universitario y de facultad y doblado</t>
+  </si>
+  <si>
+    <t>5202 impresiones papel TA4 bond a 1 solo color, corte y doblado a 0.20 c/u</t>
+  </si>
+  <si>
+    <t>200 impresiones TA3 couche 150 gramos a 3 soles c/u + 75 plastificado</t>
+  </si>
+  <si>
+    <t>200 hojas enumeradas TA3 a 1 solo color a 0.10 soles c/u</t>
+  </si>
+  <si>
+    <t>780 hojas enumeradas TA3 a 1 solo color a 0.10 c/u</t>
+  </si>
+  <si>
+    <t>49 certificados TA4 a full color con cartulina de hilo a 2 soles c/u</t>
+  </si>
+  <si>
+    <t>3 impresiones TA3 a full color, couche 200 a 3 soles cada uno</t>
+  </si>
+  <si>
+    <t>6 fotos TA4 a full color</t>
+  </si>
+  <si>
+    <t>al 153,444</t>
+  </si>
+  <si>
+    <t>al 153,447</t>
+  </si>
+  <si>
+    <t>al 153,496</t>
+  </si>
+  <si>
+    <t>al 154,276</t>
+  </si>
+  <si>
+    <t>al 154,376</t>
+  </si>
+  <si>
+    <t>al 154,575</t>
+  </si>
+  <si>
+    <t>al 159,780</t>
+  </si>
+  <si>
+    <t>oficio 144 - 2011 - OGBU/UNCP</t>
+  </si>
+  <si>
+    <t>corte de cartulinas</t>
+  </si>
+  <si>
+    <t>corte de 7 cartulinas modelo carnet</t>
   </si>
 </sst>
 </file>
@@ -7185,10 +7275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J662"/>
+  <dimension ref="A1:J670"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A515" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A529" sqref="A529"/>
+    <sheetView tabSelected="1" topLeftCell="H641" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J666" sqref="J666"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -22638,328 +22728,344 @@
         <v>468</v>
       </c>
       <c r="E529" s="2" t="s">
+        <v>2256</v>
+      </c>
+      <c r="F529" s="2" t="s">
         <v>2252</v>
       </c>
-      <c r="F529" s="2" t="s">
+      <c r="G529" s="2" t="s">
         <v>2253</v>
       </c>
-      <c r="G529" s="2" t="s">
+      <c r="H529" s="2" t="s">
         <v>2254</v>
       </c>
-      <c r="H529" s="2" t="s">
+      <c r="I529" s="2" t="s">
         <v>2255</v>
-      </c>
-      <c r="I529" s="2" t="s">
-        <v>2256</v>
       </c>
       <c r="J529" s="6">
         <v>225</v>
       </c>
     </row>
-    <row r="530" spans="1:10" s="1" customFormat="1">
+    <row r="530" spans="1:10">
       <c r="A530" s="8" t="s">
-        <v>1609</v>
+        <v>668</v>
       </c>
       <c r="B530" s="2"/>
       <c r="C530" s="3">
-        <v>40546</v>
-      </c>
-      <c r="D530" s="8" t="s">
-        <v>468</v>
-      </c>
-      <c r="E530" s="8" t="s">
-        <v>1610</v>
-      </c>
-      <c r="F530" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="G530" s="8" t="s">
-        <v>1611</v>
-      </c>
-      <c r="H530" s="8" t="s">
-        <v>1612</v>
-      </c>
-      <c r="I530" s="2"/>
+        <v>40865</v>
+      </c>
+      <c r="D530" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="E530" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="F530" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="G530" s="2" t="s">
+        <v>2264</v>
+      </c>
+      <c r="H530" s="2" t="s">
+        <v>2276</v>
+      </c>
+      <c r="I530" s="2" t="s">
+        <v>2277</v>
+      </c>
       <c r="J530" s="6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="531" spans="1:10" s="1" customFormat="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="531" spans="1:10">
       <c r="A531" s="8" t="s">
-        <v>1609</v>
+        <v>668</v>
       </c>
       <c r="B531" s="2"/>
       <c r="C531" s="3">
-        <v>40633</v>
-      </c>
-      <c r="D531" s="8" t="s">
-        <v>468</v>
-      </c>
-      <c r="E531" s="8" t="s">
-        <v>1613</v>
-      </c>
-      <c r="F531" s="8" t="s">
-        <v>1614</v>
-      </c>
-      <c r="G531" s="8" t="s">
-        <v>1615</v>
-      </c>
-      <c r="H531" s="8" t="s">
-        <v>1616</v>
-      </c>
-      <c r="I531" s="2"/>
+        <v>40865</v>
+      </c>
+      <c r="D531" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E531" s="2" t="s">
+        <v>2257</v>
+      </c>
+      <c r="F531" s="2" t="s">
+        <v>2047</v>
+      </c>
+      <c r="G531" s="2" t="s">
+        <v>2265</v>
+      </c>
+      <c r="H531" s="2" t="s">
+        <v>2275</v>
+      </c>
+      <c r="I531" s="2" t="s">
+        <v>2278</v>
+      </c>
       <c r="J531" s="6">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="532" spans="1:10" s="1" customFormat="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="532" spans="1:10">
       <c r="A532" s="8" t="s">
-        <v>1609</v>
+        <v>668</v>
       </c>
       <c r="B532" s="2"/>
       <c r="C532" s="3">
-        <v>40812</v>
-      </c>
-      <c r="D532" s="8" t="s">
-        <v>468</v>
-      </c>
-      <c r="E532" s="8" t="s">
-        <v>2002</v>
-      </c>
-      <c r="F532" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G532" s="8" t="s">
-        <v>2003</v>
-      </c>
-      <c r="H532" s="8" t="s">
-        <v>2004</v>
-      </c>
-      <c r="I532" s="2"/>
+        <v>40865</v>
+      </c>
+      <c r="D532" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E532" s="2" t="s">
+        <v>2258</v>
+      </c>
+      <c r="F532" s="2" t="s">
+        <v>2262</v>
+      </c>
+      <c r="G532" s="2" t="s">
+        <v>2266</v>
+      </c>
+      <c r="H532" s="2" t="s">
+        <v>2274</v>
+      </c>
+      <c r="I532" s="2" t="s">
+        <v>2279</v>
+      </c>
       <c r="J532" s="6">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="533" spans="1:10" s="1" customFormat="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="533" spans="1:10">
       <c r="A533" s="8" t="s">
-        <v>1609</v>
+        <v>668</v>
       </c>
       <c r="B533" s="2"/>
       <c r="C533" s="3">
-        <v>40828</v>
-      </c>
-      <c r="D533" s="8" t="s">
-        <v>468</v>
-      </c>
-      <c r="E533" s="8" t="s">
-        <v>2064</v>
-      </c>
-      <c r="F533" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G533" s="8" t="s">
-        <v>2065</v>
-      </c>
-      <c r="H533" s="8" t="s">
-        <v>2066</v>
-      </c>
-      <c r="I533" s="2"/>
+        <v>40865</v>
+      </c>
+      <c r="D533" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E533" s="2" t="s">
+        <v>2259</v>
+      </c>
+      <c r="F533" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G533" s="2" t="s">
+        <v>2267</v>
+      </c>
+      <c r="H533" s="2" t="s">
+        <v>2273</v>
+      </c>
+      <c r="I533" s="2" t="s">
+        <v>2280</v>
+      </c>
       <c r="J533" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="534" spans="1:10" s="1" customFormat="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="534" spans="1:10">
       <c r="A534" s="8" t="s">
-        <v>1617</v>
+        <v>668</v>
       </c>
       <c r="B534" s="2"/>
       <c r="C534" s="3">
-        <v>40185</v>
-      </c>
-      <c r="D534" s="8" t="s">
-        <v>468</v>
-      </c>
-      <c r="E534" s="8" t="s">
-        <v>1618</v>
-      </c>
-      <c r="F534" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G534" s="8" t="s">
-        <v>1752</v>
-      </c>
-      <c r="H534" s="8" t="s">
-        <v>1753</v>
-      </c>
-      <c r="I534" s="2"/>
+        <v>40865</v>
+      </c>
+      <c r="D534" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E534" s="2" t="s">
+        <v>2259</v>
+      </c>
+      <c r="F534" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G534" s="2" t="s">
+        <v>2267</v>
+      </c>
+      <c r="H534" s="2" t="s">
+        <v>2272</v>
+      </c>
+      <c r="I534" s="2" t="s">
+        <v>2281</v>
+      </c>
       <c r="J534" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="535" spans="1:10" s="1" customFormat="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="535" spans="1:10">
       <c r="A535" s="8" t="s">
-        <v>1617</v>
+        <v>668</v>
       </c>
       <c r="B535" s="2"/>
       <c r="C535" s="3">
-        <v>40190</v>
-      </c>
-      <c r="D535" s="8" t="s">
-        <v>468</v>
-      </c>
-      <c r="E535" s="8" t="s">
-        <v>1619</v>
-      </c>
-      <c r="F535" s="8" t="s">
-        <v>1620</v>
-      </c>
-      <c r="G535" s="8" t="s">
-        <v>1754</v>
-      </c>
-      <c r="H535" s="8" t="s">
-        <v>1755</v>
-      </c>
-      <c r="I535" s="2"/>
+        <v>40868</v>
+      </c>
+      <c r="D535" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E535" s="2" t="s">
+        <v>2260</v>
+      </c>
+      <c r="F535" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G535" s="2" t="s">
+        <v>2268</v>
+      </c>
+      <c r="H535" s="2" t="s">
+        <v>2271</v>
+      </c>
+      <c r="I535" s="2" t="s">
+        <v>2282</v>
+      </c>
       <c r="J535" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="536" spans="1:10" s="1" customFormat="1">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="536" spans="1:10">
       <c r="A536" s="8" t="s">
-        <v>1617</v>
+        <v>668</v>
       </c>
       <c r="B536" s="2"/>
       <c r="C536" s="3">
-        <v>40191</v>
-      </c>
-      <c r="D536" s="8" t="s">
-        <v>470</v>
-      </c>
-      <c r="E536" s="8" t="s">
-        <v>1621</v>
-      </c>
-      <c r="F536" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G536" s="8" t="s">
-        <v>1756</v>
-      </c>
-      <c r="H536" s="8" t="s">
-        <v>1757</v>
-      </c>
-      <c r="I536" s="2"/>
+        <v>40868</v>
+      </c>
+      <c r="D536" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E536" s="2" t="s">
+        <v>2261</v>
+      </c>
+      <c r="F536" s="2" t="s">
+        <v>2263</v>
+      </c>
+      <c r="G536" s="2" t="s">
+        <v>2269</v>
+      </c>
+      <c r="H536" s="2" t="s">
+        <v>2270</v>
+      </c>
+      <c r="I536" s="2" t="s">
+        <v>2283</v>
+      </c>
       <c r="J536" s="6">
-        <v>2</v>
+        <v>1040.4000000000001</v>
       </c>
     </row>
     <row r="537" spans="1:10" s="1" customFormat="1">
       <c r="A537" s="8" t="s">
-        <v>1617</v>
+        <v>1609</v>
       </c>
       <c r="B537" s="2"/>
       <c r="C537" s="3">
-        <v>40198</v>
+        <v>40546</v>
       </c>
       <c r="D537" s="8" t="s">
         <v>468</v>
       </c>
       <c r="E537" s="8" t="s">
-        <v>1622</v>
+        <v>1610</v>
       </c>
       <c r="F537" s="8" t="s">
-        <v>1623</v>
+        <v>479</v>
       </c>
       <c r="G537" s="8" t="s">
-        <v>1754</v>
+        <v>1611</v>
       </c>
       <c r="H537" s="8" t="s">
-        <v>1758</v>
+        <v>1612</v>
       </c>
       <c r="I537" s="2"/>
       <c r="J537" s="6">
-        <v>2</v>
+        <v>50</v>
       </c>
     </row>
     <row r="538" spans="1:10" s="1" customFormat="1">
       <c r="A538" s="8" t="s">
-        <v>1617</v>
+        <v>1609</v>
       </c>
       <c r="B538" s="2"/>
       <c r="C538" s="3">
-        <v>40203</v>
+        <v>40633</v>
       </c>
       <c r="D538" s="8" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E538" s="8" t="s">
-        <v>977</v>
+        <v>1613</v>
       </c>
       <c r="F538" s="8" t="s">
-        <v>1624</v>
+        <v>1614</v>
       </c>
       <c r="G538" s="8" t="s">
-        <v>1759</v>
+        <v>1615</v>
       </c>
       <c r="H538" s="8" t="s">
-        <v>1760</v>
+        <v>1616</v>
       </c>
       <c r="I538" s="2"/>
       <c r="J538" s="6">
-        <v>2</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="539" spans="1:10" s="1" customFormat="1">
       <c r="A539" s="8" t="s">
-        <v>1617</v>
+        <v>1609</v>
       </c>
       <c r="B539" s="2"/>
       <c r="C539" s="3">
-        <v>40206</v>
+        <v>40812</v>
       </c>
       <c r="D539" s="8" t="s">
         <v>468</v>
       </c>
       <c r="E539" s="8" t="s">
-        <v>1625</v>
+        <v>2002</v>
       </c>
       <c r="F539" s="8" t="s">
-        <v>1626</v>
+        <v>70</v>
       </c>
       <c r="G539" s="8" t="s">
-        <v>1761</v>
+        <v>2003</v>
       </c>
       <c r="H539" s="8" t="s">
-        <v>1762</v>
+        <v>2004</v>
       </c>
       <c r="I539" s="2"/>
       <c r="J539" s="6">
-        <v>3</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="540" spans="1:10" s="1" customFormat="1">
       <c r="A540" s="8" t="s">
-        <v>1617</v>
+        <v>1609</v>
       </c>
       <c r="B540" s="2"/>
       <c r="C540" s="3">
-        <v>40213</v>
-      </c>
-      <c r="D540" s="2"/>
+        <v>40828</v>
+      </c>
+      <c r="D540" s="8" t="s">
+        <v>468</v>
+      </c>
       <c r="E540" s="8" t="s">
-        <v>1628</v>
+        <v>2064</v>
       </c>
       <c r="F540" s="8" t="s">
-        <v>1629</v>
+        <v>70</v>
       </c>
       <c r="G540" s="8" t="s">
-        <v>1763</v>
+        <v>2065</v>
       </c>
       <c r="H540" s="8" t="s">
-        <v>1916</v>
+        <v>2066</v>
       </c>
       <c r="I540" s="2"/>
       <c r="J540" s="6">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="541" spans="1:10" s="1" customFormat="1">
@@ -22968,19 +23074,27 @@
       </c>
       <c r="B541" s="2"/>
       <c r="C541" s="3">
-        <v>40213</v>
+        <v>40185</v>
       </c>
       <c r="D541" s="8" t="s">
-        <v>913</v>
-      </c>
-      <c r="E541" s="2"/>
-      <c r="F541" s="2"/>
+        <v>468</v>
+      </c>
+      <c r="E541" s="8" t="s">
+        <v>1618</v>
+      </c>
+      <c r="F541" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="G541" s="8" t="s">
-        <v>1764</v>
-      </c>
-      <c r="H541" s="2"/>
+        <v>1752</v>
+      </c>
+      <c r="H541" s="8" t="s">
+        <v>1753</v>
+      </c>
       <c r="I541" s="2"/>
-      <c r="J541" s="6"/>
+      <c r="J541" s="6">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="542" spans="1:10" s="1" customFormat="1">
       <c r="A542" s="8" t="s">
@@ -22988,22 +23102,22 @@
       </c>
       <c r="B542" s="2"/>
       <c r="C542" s="3">
-        <v>40218</v>
-      </c>
-      <c r="D542" s="2" t="s">
-        <v>977</v>
+        <v>40190</v>
+      </c>
+      <c r="D542" s="8" t="s">
+        <v>468</v>
       </c>
       <c r="E542" s="8" t="s">
-        <v>977</v>
+        <v>1619</v>
       </c>
       <c r="F542" s="8" t="s">
-        <v>1630</v>
+        <v>1620</v>
       </c>
       <c r="G542" s="8" t="s">
-        <v>1765</v>
+        <v>1754</v>
       </c>
       <c r="H542" s="8" t="s">
-        <v>1766</v>
+        <v>1755</v>
       </c>
       <c r="I542" s="2"/>
       <c r="J542" s="6">
@@ -23016,26 +23130,26 @@
       </c>
       <c r="B543" s="2"/>
       <c r="C543" s="3">
-        <v>40234</v>
-      </c>
-      <c r="D543" s="2" t="s">
-        <v>468</v>
+        <v>40191</v>
+      </c>
+      <c r="D543" s="8" t="s">
+        <v>470</v>
       </c>
       <c r="E543" s="8" t="s">
-        <v>1631</v>
+        <v>1621</v>
       </c>
       <c r="F543" s="8" t="s">
-        <v>478</v>
+        <v>30</v>
       </c>
       <c r="G543" s="8" t="s">
-        <v>1768</v>
+        <v>1756</v>
       </c>
       <c r="H543" s="8" t="s">
-        <v>1769</v>
+        <v>1757</v>
       </c>
       <c r="I543" s="2"/>
       <c r="J543" s="6">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="544" spans="1:10" s="1" customFormat="1">
@@ -23044,26 +23158,26 @@
       </c>
       <c r="B544" s="2"/>
       <c r="C544" s="3">
-        <v>40239</v>
-      </c>
-      <c r="D544" s="2" t="s">
+        <v>40198</v>
+      </c>
+      <c r="D544" s="8" t="s">
         <v>468</v>
       </c>
       <c r="E544" s="8" t="s">
-        <v>1632</v>
+        <v>1622</v>
       </c>
       <c r="F544" s="8" t="s">
-        <v>1633</v>
+        <v>1623</v>
       </c>
       <c r="G544" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H544" s="8" t="s">
-        <v>1771</v>
+        <v>1758</v>
       </c>
       <c r="I544" s="2"/>
       <c r="J544" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="545" spans="1:10" s="1" customFormat="1">
@@ -23072,26 +23186,26 @@
       </c>
       <c r="B545" s="2"/>
       <c r="C545" s="3">
-        <v>40246</v>
-      </c>
-      <c r="D545" s="2" t="s">
-        <v>468</v>
+        <v>40203</v>
+      </c>
+      <c r="D545" s="8" t="s">
+        <v>977</v>
       </c>
       <c r="E545" s="8" t="s">
-        <v>1634</v>
+        <v>977</v>
       </c>
       <c r="F545" s="8" t="s">
-        <v>1635</v>
+        <v>1624</v>
       </c>
       <c r="G545" s="8" t="s">
-        <v>1754</v>
+        <v>1759</v>
       </c>
       <c r="H545" s="8" t="s">
-        <v>1772</v>
+        <v>1760</v>
       </c>
       <c r="I545" s="2"/>
       <c r="J545" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="546" spans="1:10" s="1" customFormat="1">
@@ -23100,26 +23214,26 @@
       </c>
       <c r="B546" s="2"/>
       <c r="C546" s="3">
-        <v>40260</v>
-      </c>
-      <c r="D546" s="2" t="s">
+        <v>40206</v>
+      </c>
+      <c r="D546" s="8" t="s">
         <v>468</v>
       </c>
       <c r="E546" s="8" t="s">
-        <v>1636</v>
+        <v>1625</v>
       </c>
       <c r="F546" s="8" t="s">
-        <v>1638</v>
+        <v>1626</v>
       </c>
       <c r="G546" s="8" t="s">
-        <v>1754</v>
+        <v>1761</v>
       </c>
       <c r="H546" s="8" t="s">
-        <v>1773</v>
+        <v>1762</v>
       </c>
       <c r="I546" s="2"/>
       <c r="J546" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="547" spans="1:10" s="1" customFormat="1">
@@ -23128,26 +23242,24 @@
       </c>
       <c r="B547" s="2"/>
       <c r="C547" s="3">
-        <v>40260</v>
-      </c>
-      <c r="D547" s="2" t="s">
-        <v>468</v>
-      </c>
+        <v>40213</v>
+      </c>
+      <c r="D547" s="2"/>
       <c r="E547" s="8" t="s">
-        <v>1637</v>
+        <v>1628</v>
       </c>
       <c r="F547" s="8" t="s">
-        <v>482</v>
+        <v>1629</v>
       </c>
       <c r="G547" s="8" t="s">
-        <v>1770</v>
+        <v>1763</v>
       </c>
       <c r="H547" s="8" t="s">
-        <v>1774</v>
+        <v>1916</v>
       </c>
       <c r="I547" s="2"/>
       <c r="J547" s="6">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="548" spans="1:10" s="1" customFormat="1">
@@ -23156,27 +23268,19 @@
       </c>
       <c r="B548" s="2"/>
       <c r="C548" s="3">
-        <v>40262</v>
-      </c>
-      <c r="D548" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="E548" s="8" t="s">
-        <v>1639</v>
-      </c>
-      <c r="F548" s="8" t="s">
-        <v>1927</v>
-      </c>
+        <v>40213</v>
+      </c>
+      <c r="D548" s="8" t="s">
+        <v>913</v>
+      </c>
+      <c r="E548" s="2"/>
+      <c r="F548" s="2"/>
       <c r="G548" s="8" t="s">
-        <v>1754</v>
-      </c>
-      <c r="H548" s="8" t="s">
-        <v>1775</v>
-      </c>
+        <v>1764</v>
+      </c>
+      <c r="H548" s="2"/>
       <c r="I548" s="2"/>
-      <c r="J548" s="6">
-        <v>1</v>
-      </c>
+      <c r="J548" s="6"/>
     </row>
     <row r="549" spans="1:10" s="1" customFormat="1">
       <c r="A549" s="8" t="s">
@@ -23184,26 +23288,26 @@
       </c>
       <c r="B549" s="2"/>
       <c r="C549" s="3">
-        <v>40262</v>
+        <v>40218</v>
       </c>
       <c r="D549" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E549" s="8" t="s">
-        <v>1640</v>
+        <v>977</v>
       </c>
       <c r="F549" s="8" t="s">
-        <v>1927</v>
+        <v>1630</v>
       </c>
       <c r="G549" s="8" t="s">
-        <v>1754</v>
+        <v>1765</v>
       </c>
       <c r="H549" s="8" t="s">
-        <v>1776</v>
+        <v>1766</v>
       </c>
       <c r="I549" s="2"/>
       <c r="J549" s="6">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="550" spans="1:10" s="1" customFormat="1">
@@ -23212,26 +23316,26 @@
       </c>
       <c r="B550" s="2"/>
       <c r="C550" s="3">
-        <v>40273</v>
+        <v>40234</v>
       </c>
       <c r="D550" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E550" s="8" t="s">
-        <v>1641</v>
+        <v>1631</v>
       </c>
       <c r="F550" s="8" t="s">
-        <v>30</v>
+        <v>478</v>
       </c>
       <c r="G550" s="8" t="s">
-        <v>1754</v>
+        <v>1768</v>
       </c>
       <c r="H550" s="8" t="s">
-        <v>1782</v>
+        <v>1769</v>
       </c>
       <c r="I550" s="2"/>
       <c r="J550" s="6">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="551" spans="1:10" s="1" customFormat="1">
@@ -23240,26 +23344,26 @@
       </c>
       <c r="B551" s="2"/>
       <c r="C551" s="3">
-        <v>40273</v>
+        <v>40239</v>
       </c>
       <c r="D551" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E551" s="8" t="s">
-        <v>1642</v>
+        <v>1632</v>
       </c>
       <c r="F551" s="8" t="s">
-        <v>1092</v>
+        <v>1633</v>
       </c>
       <c r="G551" s="8" t="s">
-        <v>1777</v>
+        <v>1754</v>
       </c>
       <c r="H551" s="8" t="s">
-        <v>1783</v>
+        <v>1771</v>
       </c>
       <c r="I551" s="2"/>
       <c r="J551" s="6">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="552" spans="1:10" s="1" customFormat="1">
@@ -23268,26 +23372,26 @@
       </c>
       <c r="B552" s="2"/>
       <c r="C552" s="3">
-        <v>40277</v>
+        <v>40246</v>
       </c>
       <c r="D552" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E552" s="8" t="s">
-        <v>1643</v>
+        <v>1634</v>
       </c>
       <c r="F552" s="8" t="s">
-        <v>996</v>
+        <v>1635</v>
       </c>
       <c r="G552" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H552" s="8" t="s">
-        <v>1784</v>
+        <v>1772</v>
       </c>
       <c r="I552" s="2"/>
       <c r="J552" s="6">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="553" spans="1:10" s="1" customFormat="1">
@@ -23296,26 +23400,26 @@
       </c>
       <c r="B553" s="2"/>
       <c r="C553" s="3">
-        <v>40281</v>
+        <v>40260</v>
       </c>
       <c r="D553" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E553" s="8" t="s">
-        <v>977</v>
+        <v>1636</v>
       </c>
       <c r="F553" s="8" t="s">
-        <v>1644</v>
+        <v>1638</v>
       </c>
       <c r="G553" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H553" s="8" t="s">
-        <v>1785</v>
+        <v>1773</v>
       </c>
       <c r="I553" s="2"/>
       <c r="J553" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="554" spans="1:10" s="1" customFormat="1">
@@ -23324,26 +23428,26 @@
       </c>
       <c r="B554" s="2"/>
       <c r="C554" s="3">
-        <v>40282</v>
+        <v>40260</v>
       </c>
       <c r="D554" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E554" s="8" t="s">
-        <v>1645</v>
+        <v>1637</v>
       </c>
       <c r="F554" s="8" t="s">
-        <v>29</v>
+        <v>482</v>
       </c>
       <c r="G554" s="8" t="s">
-        <v>1754</v>
+        <v>1770</v>
       </c>
       <c r="H554" s="8" t="s">
-        <v>1786</v>
+        <v>1774</v>
       </c>
       <c r="I554" s="2"/>
       <c r="J554" s="6">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="555" spans="1:10" s="1" customFormat="1">
@@ -23352,26 +23456,26 @@
       </c>
       <c r="B555" s="2"/>
       <c r="C555" s="3">
-        <v>40282</v>
+        <v>40262</v>
       </c>
       <c r="D555" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E555" s="8" t="s">
-        <v>977</v>
+        <v>1639</v>
       </c>
       <c r="F555" s="8" t="s">
-        <v>1646</v>
+        <v>1927</v>
       </c>
       <c r="G555" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H555" s="8" t="s">
-        <v>1787</v>
+        <v>1775</v>
       </c>
       <c r="I555" s="2"/>
       <c r="J555" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="556" spans="1:10" s="1" customFormat="1">
@@ -23380,26 +23484,26 @@
       </c>
       <c r="B556" s="2"/>
       <c r="C556" s="3">
-        <v>40316</v>
+        <v>40262</v>
       </c>
       <c r="D556" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E556" s="8" t="s">
-        <v>1647</v>
+        <v>1640</v>
       </c>
       <c r="F556" s="8" t="s">
-        <v>1635</v>
+        <v>1927</v>
       </c>
       <c r="G556" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H556" s="8" t="s">
-        <v>1788</v>
+        <v>1776</v>
       </c>
       <c r="I556" s="2"/>
       <c r="J556" s="6">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="557" spans="1:10" s="1" customFormat="1">
@@ -23408,26 +23512,26 @@
       </c>
       <c r="B557" s="2"/>
       <c r="C557" s="3">
-        <v>40324</v>
+        <v>40273</v>
       </c>
       <c r="D557" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E557" s="8" t="s">
-        <v>1648</v>
-      </c>
-      <c r="F557" s="2" t="s">
-        <v>1733</v>
+        <v>1641</v>
+      </c>
+      <c r="F557" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="G557" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H557" s="8" t="s">
-        <v>1789</v>
+        <v>1782</v>
       </c>
       <c r="I557" s="2"/>
       <c r="J557" s="6">
-        <v>3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="558" spans="1:10" s="1" customFormat="1">
@@ -23436,26 +23540,26 @@
       </c>
       <c r="B558" s="2"/>
       <c r="C558" s="3">
-        <v>40330</v>
+        <v>40273</v>
       </c>
       <c r="D558" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E558" s="8" t="s">
-        <v>1649</v>
+        <v>1642</v>
       </c>
       <c r="F558" s="8" t="s">
-        <v>82</v>
+        <v>1092</v>
       </c>
       <c r="G558" s="8" t="s">
-        <v>1754</v>
+        <v>1777</v>
       </c>
       <c r="H558" s="8" t="s">
-        <v>1790</v>
+        <v>1783</v>
       </c>
       <c r="I558" s="2"/>
       <c r="J558" s="6">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="559" spans="1:10" s="1" customFormat="1">
@@ -23464,22 +23568,22 @@
       </c>
       <c r="B559" s="2"/>
       <c r="C559" s="3">
-        <v>40346</v>
+        <v>40277</v>
       </c>
       <c r="D559" s="2" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E559" s="8" t="s">
-        <v>1650</v>
+        <v>1643</v>
       </c>
       <c r="F559" s="8" t="s">
-        <v>1657</v>
+        <v>996</v>
       </c>
       <c r="G559" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H559" s="8" t="s">
-        <v>1791</v>
+        <v>1784</v>
       </c>
       <c r="I559" s="2"/>
       <c r="J559" s="6">
@@ -23492,26 +23596,26 @@
       </c>
       <c r="B560" s="2"/>
       <c r="C560" s="3">
-        <v>40350</v>
+        <v>40281</v>
       </c>
       <c r="D560" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E560" s="8" t="s">
-        <v>1651</v>
-      </c>
-      <c r="F560" s="2" t="s">
-        <v>1633</v>
+        <v>977</v>
+      </c>
+      <c r="F560" s="8" t="s">
+        <v>1644</v>
       </c>
       <c r="G560" s="8" t="s">
-        <v>1778</v>
+        <v>1754</v>
       </c>
       <c r="H560" s="8" t="s">
-        <v>1792</v>
+        <v>1785</v>
       </c>
       <c r="I560" s="2"/>
       <c r="J560" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="561" spans="1:10" s="1" customFormat="1">
@@ -23520,22 +23624,22 @@
       </c>
       <c r="B561" s="2"/>
       <c r="C561" s="3">
-        <v>40353</v>
+        <v>40282</v>
       </c>
       <c r="D561" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E561" s="8" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F561" s="2" t="s">
-        <v>1927</v>
+        <v>1645</v>
+      </c>
+      <c r="F561" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="G561" s="8" t="s">
-        <v>1779</v>
+        <v>1754</v>
       </c>
       <c r="H561" s="8" t="s">
-        <v>1793</v>
+        <v>1786</v>
       </c>
       <c r="I561" s="2"/>
       <c r="J561" s="6">
@@ -23548,26 +23652,26 @@
       </c>
       <c r="B562" s="2"/>
       <c r="C562" s="3">
-        <v>40368</v>
+        <v>40282</v>
       </c>
       <c r="D562" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E562" s="8" t="s">
-        <v>1653</v>
-      </c>
-      <c r="F562" s="2" t="s">
-        <v>484</v>
+        <v>977</v>
+      </c>
+      <c r="F562" s="8" t="s">
+        <v>1646</v>
       </c>
       <c r="G562" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H562" s="8" t="s">
-        <v>1794</v>
+        <v>1787</v>
       </c>
       <c r="I562" s="2"/>
       <c r="J562" s="6">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="563" spans="1:10" s="1" customFormat="1">
@@ -23576,22 +23680,22 @@
       </c>
       <c r="B563" s="2"/>
       <c r="C563" s="3">
-        <v>40372</v>
+        <v>40316</v>
       </c>
       <c r="D563" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E563" s="8" t="s">
-        <v>1654</v>
-      </c>
-      <c r="F563" s="2" t="s">
-        <v>506</v>
+        <v>1647</v>
+      </c>
+      <c r="F563" s="8" t="s">
+        <v>1635</v>
       </c>
       <c r="G563" s="8" t="s">
-        <v>1780</v>
+        <v>1754</v>
       </c>
       <c r="H563" s="8" t="s">
-        <v>1795</v>
+        <v>1788</v>
       </c>
       <c r="I563" s="2"/>
       <c r="J563" s="6">
@@ -23604,26 +23708,26 @@
       </c>
       <c r="B564" s="2"/>
       <c r="C564" s="3">
-        <v>40373</v>
+        <v>40324</v>
       </c>
       <c r="D564" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E564" s="8" t="s">
-        <v>1655</v>
+        <v>1648</v>
       </c>
       <c r="F564" s="2" t="s">
-        <v>1633</v>
+        <v>1733</v>
       </c>
       <c r="G564" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H564" s="8" t="s">
-        <v>1796</v>
+        <v>1789</v>
       </c>
       <c r="I564" s="2"/>
       <c r="J564" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="565" spans="1:10" s="1" customFormat="1">
@@ -23632,26 +23736,26 @@
       </c>
       <c r="B565" s="2"/>
       <c r="C565" s="3">
-        <v>40375</v>
+        <v>40330</v>
       </c>
       <c r="D565" s="2" t="s">
-        <v>977</v>
+        <v>470</v>
       </c>
       <c r="E565" s="8" t="s">
-        <v>977</v>
-      </c>
-      <c r="F565" s="2" t="s">
-        <v>1656</v>
+        <v>1649</v>
+      </c>
+      <c r="F565" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="G565" s="8" t="s">
-        <v>1781</v>
+        <v>1754</v>
       </c>
       <c r="H565" s="8" t="s">
-        <v>1797</v>
+        <v>1790</v>
       </c>
       <c r="I565" s="2"/>
       <c r="J565" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="566" spans="1:10" s="1" customFormat="1">
@@ -23660,26 +23764,26 @@
       </c>
       <c r="B566" s="2"/>
       <c r="C566" s="3">
-        <v>40375</v>
+        <v>40346</v>
       </c>
       <c r="D566" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E566" s="8" t="s">
-        <v>1658</v>
-      </c>
-      <c r="F566" s="2" t="s">
-        <v>1672</v>
+        <v>1650</v>
+      </c>
+      <c r="F566" s="8" t="s">
+        <v>1657</v>
       </c>
       <c r="G566" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H566" s="8" t="s">
-        <v>1800</v>
+        <v>1791</v>
       </c>
       <c r="I566" s="2"/>
       <c r="J566" s="6">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="567" spans="1:10" s="1" customFormat="1">
@@ -23688,26 +23792,26 @@
       </c>
       <c r="B567" s="2"/>
       <c r="C567" s="3">
-        <v>40382</v>
+        <v>40350</v>
       </c>
       <c r="D567" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E567" s="8" t="s">
-        <v>1659</v>
+        <v>1651</v>
       </c>
       <c r="F567" s="2" t="s">
-        <v>1734</v>
+        <v>1633</v>
       </c>
       <c r="G567" s="8" t="s">
-        <v>1798</v>
+        <v>1778</v>
       </c>
       <c r="H567" s="8" t="s">
-        <v>1801</v>
+        <v>1792</v>
       </c>
       <c r="I567" s="2"/>
       <c r="J567" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="568" spans="1:10" s="1" customFormat="1">
@@ -23716,26 +23820,26 @@
       </c>
       <c r="B568" s="2"/>
       <c r="C568" s="3">
-        <v>40382</v>
+        <v>40353</v>
       </c>
       <c r="D568" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E568" s="8" t="s">
-        <v>1660</v>
+        <v>1652</v>
       </c>
       <c r="F568" s="2" t="s">
-        <v>1735</v>
+        <v>1927</v>
       </c>
       <c r="G568" s="8" t="s">
-        <v>1798</v>
+        <v>1779</v>
       </c>
       <c r="H568" s="8" t="s">
-        <v>1802</v>
+        <v>1793</v>
       </c>
       <c r="I568" s="2"/>
       <c r="J568" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="569" spans="1:10" s="1" customFormat="1">
@@ -23744,26 +23848,26 @@
       </c>
       <c r="B569" s="2"/>
       <c r="C569" s="3">
-        <v>40386</v>
+        <v>40368</v>
       </c>
       <c r="D569" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E569" s="8" t="s">
-        <v>1661</v>
+        <v>1653</v>
       </c>
       <c r="F569" s="2" t="s">
-        <v>82</v>
+        <v>484</v>
       </c>
       <c r="G569" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H569" s="8" t="s">
-        <v>1803</v>
+        <v>1794</v>
       </c>
       <c r="I569" s="2"/>
       <c r="J569" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="570" spans="1:10" s="1" customFormat="1">
@@ -23772,26 +23876,26 @@
       </c>
       <c r="B570" s="2"/>
       <c r="C570" s="3">
-        <v>40392</v>
+        <v>40372</v>
       </c>
       <c r="D570" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E570" s="8" t="s">
-        <v>1662</v>
+        <v>1654</v>
       </c>
       <c r="F570" s="2" t="s">
-        <v>494</v>
+        <v>506</v>
       </c>
       <c r="G570" s="8" t="s">
-        <v>1754</v>
+        <v>1780</v>
       </c>
       <c r="H570" s="8" t="s">
-        <v>1804</v>
+        <v>1795</v>
       </c>
       <c r="I570" s="2"/>
       <c r="J570" s="6">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="571" spans="1:10" s="1" customFormat="1">
@@ -23800,26 +23904,26 @@
       </c>
       <c r="B571" s="2"/>
       <c r="C571" s="3">
-        <v>40393</v>
+        <v>40373</v>
       </c>
       <c r="D571" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E571" s="8" t="s">
-        <v>1663</v>
+        <v>1655</v>
       </c>
       <c r="F571" s="2" t="s">
-        <v>1927</v>
+        <v>1633</v>
       </c>
       <c r="G571" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H571" s="8" t="s">
-        <v>1805</v>
+        <v>1796</v>
       </c>
       <c r="I571" s="2"/>
       <c r="J571" s="6">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="572" spans="1:10" s="1" customFormat="1">
@@ -23828,7 +23932,7 @@
       </c>
       <c r="B572" s="2"/>
       <c r="C572" s="3">
-        <v>40399</v>
+        <v>40375</v>
       </c>
       <c r="D572" s="2" t="s">
         <v>977</v>
@@ -23837,17 +23941,17 @@
         <v>977</v>
       </c>
       <c r="F572" s="2" t="s">
-        <v>1673</v>
+        <v>1656</v>
       </c>
       <c r="G572" s="8" t="s">
-        <v>1754</v>
+        <v>1781</v>
       </c>
       <c r="H572" s="8" t="s">
-        <v>1806</v>
+        <v>1797</v>
       </c>
       <c r="I572" s="2"/>
       <c r="J572" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="573" spans="1:10" s="1" customFormat="1">
@@ -23856,26 +23960,26 @@
       </c>
       <c r="B573" s="2"/>
       <c r="C573" s="3">
-        <v>40399</v>
+        <v>40375</v>
       </c>
       <c r="D573" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E573" s="8" t="s">
-        <v>1664</v>
+        <v>1658</v>
       </c>
       <c r="F573" s="2" t="s">
-        <v>1633</v>
+        <v>1672</v>
       </c>
       <c r="G573" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H573" s="8" t="s">
-        <v>1807</v>
+        <v>1800</v>
       </c>
       <c r="I573" s="2"/>
       <c r="J573" s="6">
-        <v>12.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="574" spans="1:10" s="1" customFormat="1">
@@ -23884,26 +23988,26 @@
       </c>
       <c r="B574" s="2"/>
       <c r="C574" s="3">
-        <v>40407</v>
+        <v>40382</v>
       </c>
       <c r="D574" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E574" s="8" t="s">
-        <v>1665</v>
+        <v>1659</v>
       </c>
       <c r="F574" s="2" t="s">
-        <v>1674</v>
+        <v>1734</v>
       </c>
       <c r="G574" s="8" t="s">
-        <v>1754</v>
+        <v>1798</v>
       </c>
       <c r="H574" s="8" t="s">
-        <v>1808</v>
+        <v>1801</v>
       </c>
       <c r="I574" s="2"/>
       <c r="J574" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="575" spans="1:10" s="1" customFormat="1">
@@ -23912,26 +24016,26 @@
       </c>
       <c r="B575" s="2"/>
       <c r="C575" s="3">
-        <v>40415</v>
+        <v>40382</v>
       </c>
       <c r="D575" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E575" s="8" t="s">
-        <v>1666</v>
+        <v>1660</v>
       </c>
       <c r="F575" s="2" t="s">
-        <v>1633</v>
+        <v>1735</v>
       </c>
       <c r="G575" s="8" t="s">
-        <v>1754</v>
+        <v>1798</v>
       </c>
       <c r="H575" s="8" t="s">
-        <v>1809</v>
+        <v>1802</v>
       </c>
       <c r="I575" s="2"/>
       <c r="J575" s="6">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="576" spans="1:10" s="1" customFormat="1">
@@ -23940,26 +24044,26 @@
       </c>
       <c r="B576" s="2"/>
       <c r="C576" s="3">
-        <v>40415</v>
+        <v>40386</v>
       </c>
       <c r="D576" s="2" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E576" s="8" t="s">
-        <v>1667</v>
+        <v>1661</v>
       </c>
       <c r="F576" s="2" t="s">
-        <v>484</v>
+        <v>82</v>
       </c>
       <c r="G576" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H576" s="8" t="s">
-        <v>1810</v>
+        <v>1803</v>
       </c>
       <c r="I576" s="2"/>
       <c r="J576" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="577" spans="1:10" s="1" customFormat="1">
@@ -23968,26 +24072,26 @@
       </c>
       <c r="B577" s="2"/>
       <c r="C577" s="3">
-        <v>40424</v>
+        <v>40392</v>
       </c>
       <c r="D577" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E577" s="8" t="s">
-        <v>1668</v>
+        <v>1662</v>
       </c>
       <c r="F577" s="2" t="s">
-        <v>1034</v>
+        <v>494</v>
       </c>
       <c r="G577" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H577" s="8" t="s">
-        <v>1811</v>
+        <v>1804</v>
       </c>
       <c r="I577" s="2"/>
       <c r="J577" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="578" spans="1:10" s="1" customFormat="1">
@@ -23996,26 +24100,26 @@
       </c>
       <c r="B578" s="2"/>
       <c r="C578" s="3">
-        <v>40429</v>
+        <v>40393</v>
       </c>
       <c r="D578" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E578" s="8" t="s">
-        <v>1669</v>
+        <v>1663</v>
       </c>
       <c r="F578" s="2" t="s">
-        <v>489</v>
+        <v>1927</v>
       </c>
       <c r="G578" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H578" s="8" t="s">
-        <v>1812</v>
+        <v>1805</v>
       </c>
       <c r="I578" s="2"/>
       <c r="J578" s="6">
-        <v>3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="579" spans="1:10" s="1" customFormat="1">
@@ -24024,7 +24128,7 @@
       </c>
       <c r="B579" s="2"/>
       <c r="C579" s="3">
-        <v>40429</v>
+        <v>40399</v>
       </c>
       <c r="D579" s="2" t="s">
         <v>977</v>
@@ -24033,17 +24137,17 @@
         <v>977</v>
       </c>
       <c r="F579" s="2" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
       <c r="G579" s="8" t="s">
-        <v>1799</v>
+        <v>1754</v>
       </c>
       <c r="H579" s="8" t="s">
-        <v>1813</v>
+        <v>1806</v>
       </c>
       <c r="I579" s="2"/>
       <c r="J579" s="6">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="580" spans="1:10" s="1" customFormat="1">
@@ -24052,26 +24156,26 @@
       </c>
       <c r="B580" s="2"/>
       <c r="C580" s="3">
-        <v>40431</v>
+        <v>40399</v>
       </c>
       <c r="D580" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E580" s="8" t="s">
-        <v>1670</v>
+        <v>1664</v>
       </c>
       <c r="F580" s="2" t="s">
-        <v>29</v>
+        <v>1633</v>
       </c>
       <c r="G580" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H580" s="8" t="s">
-        <v>1814</v>
+        <v>1807</v>
       </c>
       <c r="I580" s="2"/>
       <c r="J580" s="6">
-        <v>1</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="581" spans="1:10" s="1" customFormat="1">
@@ -24080,22 +24184,22 @@
       </c>
       <c r="B581" s="2"/>
       <c r="C581" s="3">
-        <v>40437</v>
+        <v>40407</v>
       </c>
       <c r="D581" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E581" s="8" t="s">
-        <v>977</v>
+        <v>1665</v>
       </c>
       <c r="F581" s="2" t="s">
-        <v>1676</v>
+        <v>1674</v>
       </c>
       <c r="G581" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H581" s="8" t="s">
-        <v>1815</v>
+        <v>1808</v>
       </c>
       <c r="I581" s="2"/>
       <c r="J581" s="6">
@@ -24108,26 +24212,26 @@
       </c>
       <c r="B582" s="2"/>
       <c r="C582" s="3">
-        <v>40437</v>
+        <v>40415</v>
       </c>
       <c r="D582" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E582" s="8" t="s">
-        <v>1671</v>
+        <v>1666</v>
       </c>
       <c r="F582" s="2" t="s">
-        <v>1677</v>
+        <v>1633</v>
       </c>
       <c r="G582" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H582" s="8" t="s">
-        <v>1816</v>
+        <v>1809</v>
       </c>
       <c r="I582" s="2"/>
       <c r="J582" s="6">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="583" spans="1:10" s="1" customFormat="1">
@@ -24136,26 +24240,26 @@
       </c>
       <c r="B583" s="2"/>
       <c r="C583" s="3">
-        <v>40445</v>
+        <v>40415</v>
       </c>
       <c r="D583" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E583" s="8" t="s">
-        <v>977</v>
+        <v>1667</v>
       </c>
       <c r="F583" s="2" t="s">
-        <v>1678</v>
+        <v>484</v>
       </c>
       <c r="G583" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H583" s="8" t="s">
-        <v>1817</v>
+        <v>1810</v>
       </c>
       <c r="I583" s="2"/>
       <c r="J583" s="6">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="584" spans="1:10" s="1" customFormat="1">
@@ -24164,22 +24268,22 @@
       </c>
       <c r="B584" s="2"/>
       <c r="C584" s="3">
-        <v>40448</v>
+        <v>40424</v>
       </c>
       <c r="D584" s="2" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E584" s="8" t="s">
-        <v>1679</v>
+        <v>1668</v>
       </c>
       <c r="F584" s="2" t="s">
-        <v>1635</v>
+        <v>1034</v>
       </c>
       <c r="G584" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H584" s="8" t="s">
-        <v>1821</v>
+        <v>1811</v>
       </c>
       <c r="I584" s="2"/>
       <c r="J584" s="6">
@@ -24192,26 +24296,26 @@
       </c>
       <c r="B585" s="2"/>
       <c r="C585" s="3">
-        <v>40465</v>
+        <v>40429</v>
       </c>
       <c r="D585" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E585" s="8" t="s">
-        <v>1680</v>
+        <v>1669</v>
       </c>
       <c r="F585" s="2" t="s">
-        <v>1633</v>
+        <v>489</v>
       </c>
       <c r="G585" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H585" s="8" t="s">
-        <v>1822</v>
+        <v>1812</v>
       </c>
       <c r="I585" s="2"/>
       <c r="J585" s="6">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="586" spans="1:10" s="1" customFormat="1">
@@ -24220,7 +24324,7 @@
       </c>
       <c r="B586" s="2"/>
       <c r="C586" s="3">
-        <v>40466</v>
+        <v>40429</v>
       </c>
       <c r="D586" s="2" t="s">
         <v>977</v>
@@ -24229,17 +24333,17 @@
         <v>977</v>
       </c>
       <c r="F586" s="2" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="G586" s="8" t="s">
-        <v>1754</v>
+        <v>1799</v>
       </c>
       <c r="H586" s="8" t="s">
-        <v>1823</v>
+        <v>1813</v>
       </c>
       <c r="I586" s="2"/>
       <c r="J586" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="587" spans="1:10" s="1" customFormat="1">
@@ -24248,22 +24352,22 @@
       </c>
       <c r="B587" s="2"/>
       <c r="C587" s="3">
-        <v>40469</v>
+        <v>40431</v>
       </c>
       <c r="D587" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E587" s="8" t="s">
-        <v>1681</v>
+        <v>1670</v>
       </c>
       <c r="F587" s="2" t="s">
-        <v>1633</v>
+        <v>29</v>
       </c>
       <c r="G587" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H587" s="8" t="s">
-        <v>1824</v>
+        <v>1814</v>
       </c>
       <c r="I587" s="2"/>
       <c r="J587" s="6">
@@ -24276,22 +24380,22 @@
       </c>
       <c r="B588" s="2"/>
       <c r="C588" s="3">
-        <v>40478</v>
+        <v>40437</v>
       </c>
       <c r="D588" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E588" s="8" t="s">
-        <v>1682</v>
+        <v>977</v>
       </c>
       <c r="F588" s="2" t="s">
-        <v>1633</v>
+        <v>1676</v>
       </c>
       <c r="G588" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H588" s="8" t="s">
-        <v>1825</v>
+        <v>1815</v>
       </c>
       <c r="I588" s="2"/>
       <c r="J588" s="6">
@@ -24304,26 +24408,26 @@
       </c>
       <c r="B589" s="2"/>
       <c r="C589" s="3">
-        <v>40480</v>
+        <v>40437</v>
       </c>
       <c r="D589" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E589" s="8" t="s">
-        <v>1683</v>
+        <v>1671</v>
       </c>
       <c r="F589" s="2" t="s">
-        <v>1633</v>
+        <v>1677</v>
       </c>
       <c r="G589" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H589" s="8" t="s">
-        <v>1826</v>
+        <v>1816</v>
       </c>
       <c r="I589" s="2"/>
       <c r="J589" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="590" spans="1:10" s="1" customFormat="1">
@@ -24332,26 +24436,26 @@
       </c>
       <c r="B590" s="2"/>
       <c r="C590" s="3">
-        <v>40505</v>
+        <v>40445</v>
       </c>
       <c r="D590" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E590" s="8" t="s">
-        <v>1684</v>
+        <v>977</v>
       </c>
       <c r="F590" s="2" t="s">
-        <v>1633</v>
+        <v>1678</v>
       </c>
       <c r="G590" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H590" s="8" t="s">
-        <v>1827</v>
+        <v>1817</v>
       </c>
       <c r="I590" s="2"/>
       <c r="J590" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="591" spans="1:10" s="1" customFormat="1">
@@ -24360,22 +24464,22 @@
       </c>
       <c r="B591" s="2"/>
       <c r="C591" s="3">
-        <v>40508</v>
+        <v>40448</v>
       </c>
       <c r="D591" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E591" s="8" t="s">
-        <v>977</v>
+        <v>1679</v>
       </c>
       <c r="F591" s="2" t="s">
-        <v>1689</v>
+        <v>1635</v>
       </c>
       <c r="G591" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H591" s="8" t="s">
-        <v>1828</v>
+        <v>1821</v>
       </c>
       <c r="I591" s="2"/>
       <c r="J591" s="6">
@@ -24388,26 +24492,26 @@
       </c>
       <c r="B592" s="2"/>
       <c r="C592" s="3">
-        <v>40513</v>
+        <v>40465</v>
       </c>
       <c r="D592" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E592" s="8" t="s">
-        <v>1685</v>
+        <v>1680</v>
       </c>
       <c r="F592" s="2" t="s">
-        <v>1690</v>
+        <v>1633</v>
       </c>
       <c r="G592" s="8" t="s">
-        <v>1818</v>
+        <v>1754</v>
       </c>
       <c r="H592" s="8" t="s">
-        <v>1829</v>
+        <v>1822</v>
       </c>
       <c r="I592" s="2"/>
       <c r="J592" s="6">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="593" spans="1:10" s="1" customFormat="1">
@@ -24416,7 +24520,7 @@
       </c>
       <c r="B593" s="2"/>
       <c r="C593" s="3">
-        <v>40518</v>
+        <v>40466</v>
       </c>
       <c r="D593" s="2" t="s">
         <v>977</v>
@@ -24425,13 +24529,13 @@
         <v>977</v>
       </c>
       <c r="F593" s="2" t="s">
-        <v>1691</v>
+        <v>1676</v>
       </c>
       <c r="G593" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H593" s="8" t="s">
-        <v>1830</v>
+        <v>1823</v>
       </c>
       <c r="I593" s="2"/>
       <c r="J593" s="6">
@@ -24444,26 +24548,26 @@
       </c>
       <c r="B594" s="2"/>
       <c r="C594" s="3">
-        <v>40518</v>
+        <v>40469</v>
       </c>
       <c r="D594" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E594" s="8" t="s">
-        <v>1686</v>
+        <v>1681</v>
       </c>
       <c r="F594" s="2" t="s">
-        <v>30</v>
+        <v>1633</v>
       </c>
       <c r="G594" s="8" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="H594" s="8" t="s">
-        <v>1831</v>
+        <v>1824</v>
       </c>
       <c r="I594" s="2"/>
       <c r="J594" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="595" spans="1:10" s="1" customFormat="1">
@@ -24472,13 +24576,13 @@
       </c>
       <c r="B595" s="2"/>
       <c r="C595" s="3">
-        <v>40518</v>
+        <v>40478</v>
       </c>
       <c r="D595" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E595" s="8" t="s">
-        <v>1687</v>
+        <v>1682</v>
       </c>
       <c r="F595" s="2" t="s">
         <v>1633</v>
@@ -24487,11 +24591,11 @@
         <v>1754</v>
       </c>
       <c r="H595" s="8" t="s">
-        <v>1832</v>
+        <v>1825</v>
       </c>
       <c r="I595" s="2"/>
       <c r="J595" s="6">
-        <v>22.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="596" spans="1:10" s="1" customFormat="1">
@@ -24500,26 +24604,26 @@
       </c>
       <c r="B596" s="2"/>
       <c r="C596" s="3">
-        <v>40522</v>
+        <v>40480</v>
       </c>
       <c r="D596" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E596" s="8" t="s">
-        <v>977</v>
+        <v>1683</v>
       </c>
       <c r="F596" s="2" t="s">
-        <v>1692</v>
+        <v>1633</v>
       </c>
       <c r="G596" s="8" t="s">
-        <v>1819</v>
+        <v>1754</v>
       </c>
       <c r="H596" s="8" t="s">
-        <v>1833</v>
+        <v>1826</v>
       </c>
       <c r="I596" s="2"/>
       <c r="J596" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="597" spans="1:10" s="1" customFormat="1">
@@ -24528,26 +24632,26 @@
       </c>
       <c r="B597" s="2"/>
       <c r="C597" s="3">
-        <v>40526</v>
+        <v>40505</v>
       </c>
       <c r="D597" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E597" s="8" t="s">
-        <v>1688</v>
+        <v>1684</v>
       </c>
       <c r="F597" s="2" t="s">
-        <v>493</v>
+        <v>1633</v>
       </c>
       <c r="G597" s="8" t="s">
-        <v>1820</v>
+        <v>1754</v>
       </c>
       <c r="H597" s="8" t="s">
-        <v>1834</v>
+        <v>1827</v>
       </c>
       <c r="I597" s="2"/>
       <c r="J597" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="598" spans="1:10" s="1" customFormat="1">
@@ -24556,26 +24660,26 @@
       </c>
       <c r="B598" s="2"/>
       <c r="C598" s="3">
-        <v>40548</v>
+        <v>40508</v>
       </c>
       <c r="D598" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E598" s="8" t="s">
-        <v>1693</v>
+        <v>977</v>
       </c>
       <c r="F598" s="2" t="s">
-        <v>493</v>
+        <v>1689</v>
       </c>
       <c r="G598" s="8" t="s">
-        <v>1835</v>
+        <v>1754</v>
       </c>
       <c r="H598" s="8" t="s">
-        <v>1839</v>
+        <v>1828</v>
       </c>
       <c r="I598" s="2"/>
       <c r="J598" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="599" spans="1:10" s="1" customFormat="1">
@@ -24584,22 +24688,22 @@
       </c>
       <c r="B599" s="2"/>
       <c r="C599" s="3">
-        <v>40553</v>
+        <v>40513</v>
       </c>
       <c r="D599" s="2" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E599" s="8" t="s">
-        <v>1694</v>
+        <v>1685</v>
       </c>
       <c r="F599" s="2" t="s">
-        <v>74</v>
+        <v>1690</v>
       </c>
       <c r="G599" s="8" t="s">
-        <v>1754</v>
+        <v>1818</v>
       </c>
       <c r="H599" s="8" t="s">
-        <v>1840</v>
+        <v>1829</v>
       </c>
       <c r="I599" s="2"/>
       <c r="J599" s="6">
@@ -24612,26 +24716,26 @@
       </c>
       <c r="B600" s="2"/>
       <c r="C600" s="3">
-        <v>40564</v>
+        <v>40518</v>
       </c>
       <c r="D600" s="2" t="s">
-        <v>470</v>
+        <v>977</v>
       </c>
       <c r="E600" s="8" t="s">
-        <v>1695</v>
+        <v>977</v>
       </c>
       <c r="F600" s="2" t="s">
-        <v>1702</v>
+        <v>1691</v>
       </c>
       <c r="G600" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H600" s="8" t="s">
-        <v>1841</v>
+        <v>1830</v>
       </c>
       <c r="I600" s="2"/>
       <c r="J600" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="601" spans="1:10" s="1" customFormat="1">
@@ -24640,26 +24744,26 @@
       </c>
       <c r="B601" s="2"/>
       <c r="C601" s="3">
-        <v>40582</v>
+        <v>40518</v>
       </c>
       <c r="D601" s="2" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E601" s="8" t="s">
-        <v>1696</v>
+        <v>1686</v>
       </c>
       <c r="F601" s="2" t="s">
-        <v>1703</v>
+        <v>30</v>
       </c>
       <c r="G601" s="8" t="s">
-        <v>1754</v>
+        <v>1756</v>
       </c>
       <c r="H601" s="8" t="s">
-        <v>1842</v>
+        <v>1831</v>
       </c>
       <c r="I601" s="2"/>
       <c r="J601" s="6">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="602" spans="1:10" s="1" customFormat="1">
@@ -24668,26 +24772,26 @@
       </c>
       <c r="B602" s="2"/>
       <c r="C602" s="3">
-        <v>40582</v>
+        <v>40518</v>
       </c>
       <c r="D602" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E602" s="8" t="s">
-        <v>977</v>
+        <v>1687</v>
       </c>
       <c r="F602" s="2" t="s">
-        <v>1704</v>
+        <v>1633</v>
       </c>
       <c r="G602" s="8" t="s">
-        <v>1836</v>
+        <v>1754</v>
       </c>
       <c r="H602" s="8" t="s">
-        <v>1843</v>
+        <v>1832</v>
       </c>
       <c r="I602" s="2"/>
       <c r="J602" s="6">
-        <v>1</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="603" spans="1:10" s="1" customFormat="1">
@@ -24696,7 +24800,7 @@
       </c>
       <c r="B603" s="2"/>
       <c r="C603" s="3">
-        <v>40595</v>
+        <v>40522</v>
       </c>
       <c r="D603" s="2" t="s">
         <v>977</v>
@@ -24705,17 +24809,17 @@
         <v>977</v>
       </c>
       <c r="F603" s="2" t="s">
-        <v>1705</v>
+        <v>1692</v>
       </c>
       <c r="G603" s="8" t="s">
-        <v>1837</v>
+        <v>1819</v>
       </c>
       <c r="H603" s="8" t="s">
-        <v>1844</v>
+        <v>1833</v>
       </c>
       <c r="I603" s="2"/>
       <c r="J603" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="604" spans="1:10" s="1" customFormat="1">
@@ -24724,26 +24828,26 @@
       </c>
       <c r="B604" s="2"/>
       <c r="C604" s="3">
-        <v>40606</v>
+        <v>40526</v>
       </c>
       <c r="D604" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E604" s="8" t="s">
-        <v>1697</v>
+        <v>1688</v>
       </c>
       <c r="F604" s="2" t="s">
-        <v>1706</v>
+        <v>493</v>
       </c>
       <c r="G604" s="8" t="s">
-        <v>1754</v>
+        <v>1820</v>
       </c>
       <c r="H604" s="8" t="s">
-        <v>1801</v>
+        <v>1834</v>
       </c>
       <c r="I604" s="2"/>
       <c r="J604" s="6">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="605" spans="1:10" s="1" customFormat="1">
@@ -24752,26 +24856,26 @@
       </c>
       <c r="B605" s="2"/>
       <c r="C605" s="3">
-        <v>40611</v>
+        <v>40548</v>
       </c>
       <c r="D605" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E605" s="8" t="s">
-        <v>977</v>
+        <v>1693</v>
       </c>
       <c r="F605" s="2" t="s">
-        <v>1707</v>
+        <v>493</v>
       </c>
       <c r="G605" s="8" t="s">
-        <v>1838</v>
+        <v>1835</v>
       </c>
       <c r="H605" s="8" t="s">
-        <v>1845</v>
+        <v>1839</v>
       </c>
       <c r="I605" s="2"/>
       <c r="J605" s="6">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="606" spans="1:10" s="1" customFormat="1">
@@ -24780,26 +24884,26 @@
       </c>
       <c r="B606" s="2"/>
       <c r="C606" s="3">
-        <v>40612</v>
+        <v>40553</v>
       </c>
       <c r="D606" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E606" s="8" t="s">
-        <v>1698</v>
+        <v>1694</v>
       </c>
       <c r="F606" s="2" t="s">
-        <v>1703</v>
+        <v>74</v>
       </c>
       <c r="G606" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H606" s="8" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
       <c r="I606" s="2"/>
       <c r="J606" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="607" spans="1:10" s="1" customFormat="1">
@@ -24808,22 +24912,22 @@
       </c>
       <c r="B607" s="2"/>
       <c r="C607" s="3">
-        <v>40618</v>
+        <v>40564</v>
       </c>
       <c r="D607" s="2" t="s">
-        <v>977</v>
+        <v>470</v>
       </c>
       <c r="E607" s="8" t="s">
-        <v>977</v>
+        <v>1695</v>
       </c>
       <c r="F607" s="2" t="s">
-        <v>1708</v>
+        <v>1702</v>
       </c>
       <c r="G607" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H607" s="8" t="s">
-        <v>1846</v>
+        <v>1841</v>
       </c>
       <c r="I607" s="2"/>
       <c r="J607" s="6">
@@ -24836,13 +24940,13 @@
       </c>
       <c r="B608" s="2"/>
       <c r="C608" s="3">
-        <v>40619</v>
+        <v>40582</v>
       </c>
       <c r="D608" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E608" s="8" t="s">
-        <v>1699</v>
+        <v>1696</v>
       </c>
       <c r="F608" s="2" t="s">
         <v>1703</v>
@@ -24851,11 +24955,11 @@
         <v>1754</v>
       </c>
       <c r="H608" s="8" t="s">
-        <v>1847</v>
+        <v>1842</v>
       </c>
       <c r="I608" s="2"/>
       <c r="J608" s="6">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="609" spans="1:10" s="1" customFormat="1">
@@ -24864,22 +24968,22 @@
       </c>
       <c r="B609" s="2"/>
       <c r="C609" s="3">
-        <v>40620</v>
+        <v>40582</v>
       </c>
       <c r="D609" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E609" s="8" t="s">
-        <v>1700</v>
+        <v>977</v>
       </c>
       <c r="F609" s="2" t="s">
-        <v>494</v>
+        <v>1704</v>
       </c>
       <c r="G609" s="8" t="s">
-        <v>1754</v>
+        <v>1836</v>
       </c>
       <c r="H609" s="8" t="s">
-        <v>1848</v>
+        <v>1843</v>
       </c>
       <c r="I609" s="2"/>
       <c r="J609" s="6">
@@ -24892,22 +24996,22 @@
       </c>
       <c r="B610" s="2"/>
       <c r="C610" s="3">
-        <v>40626</v>
+        <v>40595</v>
       </c>
       <c r="D610" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E610" s="8" t="s">
-        <v>1701</v>
+        <v>977</v>
       </c>
       <c r="F610" s="2" t="s">
-        <v>1635</v>
+        <v>1705</v>
       </c>
       <c r="G610" s="8" t="s">
-        <v>1754</v>
+        <v>1837</v>
       </c>
       <c r="H610" s="8" t="s">
-        <v>1849</v>
+        <v>1844</v>
       </c>
       <c r="I610" s="2"/>
       <c r="J610" s="6">
@@ -24920,26 +25024,26 @@
       </c>
       <c r="B611" s="2"/>
       <c r="C611" s="3">
-        <v>40632</v>
+        <v>40606</v>
       </c>
       <c r="D611" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E611" s="8" t="s">
-        <v>977</v>
+        <v>1697</v>
       </c>
       <c r="F611" s="2" t="s">
-        <v>1709</v>
+        <v>1706</v>
       </c>
       <c r="G611" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H611" s="8" t="s">
-        <v>1850</v>
+        <v>1801</v>
       </c>
       <c r="I611" s="2"/>
       <c r="J611" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="612" spans="1:10" s="1" customFormat="1">
@@ -24948,7 +25052,7 @@
       </c>
       <c r="B612" s="2"/>
       <c r="C612" s="3">
-        <v>40632</v>
+        <v>40611</v>
       </c>
       <c r="D612" s="2" t="s">
         <v>977</v>
@@ -24957,17 +25061,17 @@
         <v>977</v>
       </c>
       <c r="F612" s="2" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="G612" s="8" t="s">
-        <v>1754</v>
+        <v>1838</v>
       </c>
       <c r="H612" s="8" t="s">
-        <v>1851</v>
+        <v>1845</v>
       </c>
       <c r="I612" s="2"/>
       <c r="J612" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="613" spans="1:10" s="1" customFormat="1">
@@ -24976,26 +25080,26 @@
       </c>
       <c r="B613" s="2"/>
       <c r="C613" s="3">
-        <v>40632</v>
+        <v>40612</v>
       </c>
       <c r="D613" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E613" s="8" t="s">
-        <v>977</v>
+        <v>1698</v>
       </c>
       <c r="F613" s="2" t="s">
-        <v>1710</v>
+        <v>1703</v>
       </c>
       <c r="G613" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H613" s="8" t="s">
-        <v>1852</v>
+        <v>1842</v>
       </c>
       <c r="I613" s="2"/>
       <c r="J613" s="6">
-        <v>0.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="614" spans="1:10" s="1" customFormat="1">
@@ -25004,7 +25108,7 @@
       </c>
       <c r="B614" s="2"/>
       <c r="C614" s="3">
-        <v>40632</v>
+        <v>40618</v>
       </c>
       <c r="D614" s="2" t="s">
         <v>977</v>
@@ -25013,17 +25117,17 @@
         <v>977</v>
       </c>
       <c r="F614" s="2" t="s">
-        <v>1711</v>
+        <v>1708</v>
       </c>
       <c r="G614" s="8" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="H614" s="8" t="s">
-        <v>1853</v>
+        <v>1846</v>
       </c>
       <c r="I614" s="2"/>
       <c r="J614" s="6">
-        <v>4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="615" spans="1:10" s="1" customFormat="1">
@@ -25032,26 +25136,26 @@
       </c>
       <c r="B615" s="2"/>
       <c r="C615" s="3">
-        <v>40632</v>
+        <v>40619</v>
       </c>
       <c r="D615" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E615" s="8" t="s">
-        <v>1712</v>
+        <v>1699</v>
       </c>
       <c r="F615" s="2" t="s">
-        <v>1713</v>
+        <v>1703</v>
       </c>
       <c r="G615" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H615" s="8" t="s">
-        <v>1854</v>
+        <v>1847</v>
       </c>
       <c r="I615" s="2"/>
       <c r="J615" s="6">
-        <v>0.5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="616" spans="1:10" s="1" customFormat="1">
@@ -25060,22 +25164,22 @@
       </c>
       <c r="B616" s="2"/>
       <c r="C616" s="3">
-        <v>40639</v>
+        <v>40620</v>
       </c>
       <c r="D616" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E616" s="8" t="s">
-        <v>977</v>
+        <v>1700</v>
       </c>
       <c r="F616" s="2" t="s">
-        <v>1726</v>
+        <v>494</v>
       </c>
       <c r="G616" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H616" s="8" t="s">
-        <v>1855</v>
+        <v>1848</v>
       </c>
       <c r="I616" s="2"/>
       <c r="J616" s="6">
@@ -25088,26 +25192,26 @@
       </c>
       <c r="B617" s="2"/>
       <c r="C617" s="3">
-        <v>40639</v>
+        <v>40626</v>
       </c>
       <c r="D617" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E617" s="8" t="s">
-        <v>977</v>
+        <v>1701</v>
       </c>
       <c r="F617" s="2" t="s">
-        <v>1727</v>
+        <v>1635</v>
       </c>
       <c r="G617" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H617" s="8" t="s">
-        <v>1856</v>
+        <v>1849</v>
       </c>
       <c r="I617" s="2"/>
       <c r="J617" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="618" spans="1:10" s="1" customFormat="1">
@@ -25116,7 +25220,7 @@
       </c>
       <c r="B618" s="2"/>
       <c r="C618" s="3">
-        <v>40644</v>
+        <v>40632</v>
       </c>
       <c r="D618" s="2" t="s">
         <v>977</v>
@@ -25125,13 +25229,13 @@
         <v>977</v>
       </c>
       <c r="F618" s="2" t="s">
-        <v>1728</v>
+        <v>1709</v>
       </c>
       <c r="G618" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H618" s="8" t="s">
-        <v>1857</v>
+        <v>1850</v>
       </c>
       <c r="I618" s="2"/>
       <c r="J618" s="6">
@@ -25144,22 +25248,22 @@
       </c>
       <c r="B619" s="2"/>
       <c r="C619" s="3">
-        <v>40646</v>
+        <v>40632</v>
       </c>
       <c r="D619" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E619" s="8" t="s">
-        <v>1714</v>
+        <v>977</v>
       </c>
       <c r="F619" s="2" t="s">
-        <v>1729</v>
+        <v>1708</v>
       </c>
       <c r="G619" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H619" s="8" t="s">
-        <v>1858</v>
+        <v>1851</v>
       </c>
       <c r="I619" s="2"/>
       <c r="J619" s="6">
@@ -25172,26 +25276,26 @@
       </c>
       <c r="B620" s="2"/>
       <c r="C620" s="3">
-        <v>40646</v>
+        <v>40632</v>
       </c>
       <c r="D620" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E620" s="8" t="s">
-        <v>1715</v>
+        <v>977</v>
       </c>
       <c r="F620" s="2" t="s">
-        <v>1730</v>
+        <v>1710</v>
       </c>
       <c r="G620" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H620" s="8" t="s">
-        <v>1859</v>
+        <v>1852</v>
       </c>
       <c r="I620" s="2"/>
       <c r="J620" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="621" spans="1:10" s="1" customFormat="1">
@@ -25200,26 +25304,26 @@
       </c>
       <c r="B621" s="2"/>
       <c r="C621" s="3">
-        <v>40651</v>
+        <v>40632</v>
       </c>
       <c r="D621" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E621" s="8" t="s">
-        <v>1716</v>
+        <v>977</v>
       </c>
       <c r="F621" s="2" t="s">
-        <v>506</v>
+        <v>1711</v>
       </c>
       <c r="G621" s="8" t="s">
-        <v>1754</v>
+        <v>1756</v>
       </c>
       <c r="H621" s="8" t="s">
-        <v>1860</v>
+        <v>1853</v>
       </c>
       <c r="I621" s="2"/>
       <c r="J621" s="6">
-        <v>0.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="622" spans="1:10" s="1" customFormat="1">
@@ -25228,26 +25332,26 @@
       </c>
       <c r="B622" s="2"/>
       <c r="C622" s="3">
-        <v>40651</v>
+        <v>40632</v>
       </c>
       <c r="D622" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E622" s="8" t="s">
-        <v>1717</v>
+        <v>1712</v>
       </c>
       <c r="F622" s="2" t="s">
-        <v>1702</v>
+        <v>1713</v>
       </c>
       <c r="G622" s="8" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="H622" s="8" t="s">
-        <v>1861</v>
+        <v>1854</v>
       </c>
       <c r="I622" s="2"/>
       <c r="J622" s="6">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="623" spans="1:10" s="1" customFormat="1">
@@ -25256,26 +25360,26 @@
       </c>
       <c r="B623" s="2"/>
       <c r="C623" s="3">
-        <v>40668</v>
+        <v>40639</v>
       </c>
       <c r="D623" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E623" s="8" t="s">
-        <v>1718</v>
+        <v>977</v>
       </c>
       <c r="F623" s="2" t="s">
-        <v>1657</v>
+        <v>1726</v>
       </c>
       <c r="G623" s="8" t="s">
-        <v>1818</v>
+        <v>1754</v>
       </c>
       <c r="H623" s="8" t="s">
-        <v>1862</v>
+        <v>1855</v>
       </c>
       <c r="I623" s="2"/>
       <c r="J623" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="624" spans="1:10" s="1" customFormat="1">
@@ -25284,26 +25388,26 @@
       </c>
       <c r="B624" s="2"/>
       <c r="C624" s="3">
-        <v>40676</v>
+        <v>40639</v>
       </c>
       <c r="D624" s="2" t="s">
-        <v>470</v>
+        <v>977</v>
       </c>
       <c r="E624" s="8" t="s">
-        <v>1719</v>
+        <v>977</v>
       </c>
       <c r="F624" s="2" t="s">
-        <v>1702</v>
+        <v>1727</v>
       </c>
       <c r="G624" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H624" s="8" t="s">
-        <v>1863</v>
+        <v>1856</v>
       </c>
       <c r="I624" s="2"/>
       <c r="J624" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="625" spans="1:10" s="1" customFormat="1">
@@ -25312,26 +25416,26 @@
       </c>
       <c r="B625" s="2"/>
       <c r="C625" s="3">
-        <v>40676</v>
+        <v>40644</v>
       </c>
       <c r="D625" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E625" s="8" t="s">
-        <v>1720</v>
+        <v>977</v>
       </c>
       <c r="F625" s="2" t="s">
-        <v>1703</v>
+        <v>1728</v>
       </c>
       <c r="G625" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H625" s="8" t="s">
-        <v>1864</v>
+        <v>1857</v>
       </c>
       <c r="I625" s="2"/>
       <c r="J625" s="6">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="626" spans="1:10" s="1" customFormat="1">
@@ -25340,26 +25444,26 @@
       </c>
       <c r="B626" s="2"/>
       <c r="C626" s="3">
-        <v>40730</v>
+        <v>40646</v>
       </c>
       <c r="D626" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E626" s="8" t="s">
-        <v>1721</v>
+        <v>1714</v>
       </c>
       <c r="F626" s="2" t="s">
-        <v>1703</v>
+        <v>1729</v>
       </c>
       <c r="G626" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H626" s="8" t="s">
-        <v>1865</v>
+        <v>1858</v>
       </c>
       <c r="I626" s="2"/>
       <c r="J626" s="6">
-        <v>7.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="627" spans="1:10" s="1" customFormat="1">
@@ -25368,22 +25472,22 @@
       </c>
       <c r="B627" s="2"/>
       <c r="C627" s="3">
-        <v>40742</v>
+        <v>40646</v>
       </c>
       <c r="D627" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E627" s="8" t="s">
-        <v>1722</v>
+        <v>1715</v>
       </c>
       <c r="F627" s="2" t="s">
-        <v>1703</v>
+        <v>1730</v>
       </c>
       <c r="G627" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H627" s="8" t="s">
-        <v>1866</v>
+        <v>1859</v>
       </c>
       <c r="I627" s="2"/>
       <c r="J627" s="6">
@@ -25396,26 +25500,26 @@
       </c>
       <c r="B628" s="2"/>
       <c r="C628" s="3">
-        <v>40749</v>
+        <v>40651</v>
       </c>
       <c r="D628" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E628" s="8" t="s">
-        <v>977</v>
+        <v>1716</v>
       </c>
       <c r="F628" s="2" t="s">
-        <v>1731</v>
+        <v>506</v>
       </c>
       <c r="G628" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H628" s="8" t="s">
-        <v>1867</v>
+        <v>1860</v>
       </c>
       <c r="I628" s="2"/>
       <c r="J628" s="6">
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="629" spans="1:10" s="1" customFormat="1">
@@ -25424,22 +25528,22 @@
       </c>
       <c r="B629" s="2"/>
       <c r="C629" s="3">
-        <v>40749</v>
+        <v>40651</v>
       </c>
       <c r="D629" s="2" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E629" s="8" t="s">
-        <v>1723</v>
+        <v>1717</v>
       </c>
       <c r="F629" s="2" t="s">
-        <v>1736</v>
+        <v>1702</v>
       </c>
       <c r="G629" s="8" t="s">
-        <v>1754</v>
+        <v>1756</v>
       </c>
       <c r="H629" s="8" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="I629" s="2"/>
       <c r="J629" s="6">
@@ -25452,13 +25556,13 @@
       </c>
       <c r="B630" s="2"/>
       <c r="C630" s="3">
-        <v>40750</v>
+        <v>40668</v>
       </c>
       <c r="D630" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E630" s="8" t="s">
-        <v>1724</v>
+        <v>1718</v>
       </c>
       <c r="F630" s="2" t="s">
         <v>1657</v>
@@ -25467,11 +25571,11 @@
         <v>1818</v>
       </c>
       <c r="H630" s="8" t="s">
-        <v>1868</v>
+        <v>1862</v>
       </c>
       <c r="I630" s="2"/>
       <c r="J630" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="631" spans="1:10" s="1" customFormat="1">
@@ -25480,26 +25584,26 @@
       </c>
       <c r="B631" s="2"/>
       <c r="C631" s="3">
-        <v>40750</v>
+        <v>40676</v>
       </c>
       <c r="D631" s="2" t="s">
         <v>470</v>
       </c>
       <c r="E631" s="8" t="s">
-        <v>1725</v>
+        <v>1719</v>
       </c>
       <c r="F631" s="2" t="s">
-        <v>1737</v>
+        <v>1702</v>
       </c>
       <c r="G631" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H631" s="8" t="s">
-        <v>1869</v>
+        <v>1863</v>
       </c>
       <c r="I631" s="2"/>
       <c r="J631" s="6">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="632" spans="1:10" s="1" customFormat="1">
@@ -25508,26 +25612,26 @@
       </c>
       <c r="B632" s="2"/>
       <c r="C632" s="3">
-        <v>40757</v>
+        <v>40676</v>
       </c>
       <c r="D632" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E632" s="8" t="s">
-        <v>1738</v>
+        <v>1720</v>
       </c>
       <c r="F632" s="2" t="s">
-        <v>1747</v>
+        <v>1703</v>
       </c>
       <c r="G632" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H632" s="8" t="s">
-        <v>1870</v>
+        <v>1864</v>
       </c>
       <c r="I632" s="2"/>
       <c r="J632" s="6">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="633" spans="1:10" s="1" customFormat="1">
@@ -25536,26 +25640,26 @@
       </c>
       <c r="B633" s="2"/>
       <c r="C633" s="3">
-        <v>40758</v>
+        <v>40730</v>
       </c>
       <c r="D633" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E633" s="8" t="s">
-        <v>1739</v>
+        <v>1721</v>
       </c>
       <c r="F633" s="2" t="s">
-        <v>15</v>
+        <v>1703</v>
       </c>
       <c r="G633" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H633" s="8" t="s">
-        <v>1871</v>
+        <v>1865</v>
       </c>
       <c r="I633" s="2"/>
       <c r="J633" s="6">
-        <v>2</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="634" spans="1:10" s="1" customFormat="1">
@@ -25564,26 +25668,26 @@
       </c>
       <c r="B634" s="2"/>
       <c r="C634" s="3">
-        <v>40759</v>
+        <v>40742</v>
       </c>
       <c r="D634" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E634" s="8" t="s">
-        <v>1740</v>
+        <v>1722</v>
       </c>
       <c r="F634" s="2" t="s">
-        <v>506</v>
+        <v>1703</v>
       </c>
       <c r="G634" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H634" s="8" t="s">
-        <v>1872</v>
+        <v>1866</v>
       </c>
       <c r="I634" s="2"/>
       <c r="J634" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="635" spans="1:10" s="1" customFormat="1">
@@ -25592,26 +25696,26 @@
       </c>
       <c r="B635" s="2"/>
       <c r="C635" s="3">
-        <v>40760</v>
+        <v>40749</v>
       </c>
       <c r="D635" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E635" s="8" t="s">
-        <v>1741</v>
+        <v>977</v>
       </c>
       <c r="F635" s="2" t="s">
-        <v>1747</v>
+        <v>1731</v>
       </c>
       <c r="G635" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H635" s="8" t="s">
-        <v>1800</v>
+        <v>1867</v>
       </c>
       <c r="I635" s="2"/>
       <c r="J635" s="6">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="636" spans="1:10" s="1" customFormat="1">
@@ -25620,26 +25724,26 @@
       </c>
       <c r="B636" s="2"/>
       <c r="C636" s="3">
-        <v>40760</v>
+        <v>40749</v>
       </c>
       <c r="D636" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E636" s="8" t="s">
-        <v>1742</v>
+        <v>1723</v>
       </c>
       <c r="F636" s="2" t="s">
-        <v>49</v>
+        <v>1736</v>
       </c>
       <c r="G636" s="8" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="H636" s="8" t="s">
-        <v>1873</v>
+        <v>1862</v>
       </c>
       <c r="I636" s="2"/>
       <c r="J636" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="637" spans="1:10" s="1" customFormat="1">
@@ -25648,22 +25752,22 @@
       </c>
       <c r="B637" s="2"/>
       <c r="C637" s="3">
-        <v>40772</v>
+        <v>40750</v>
       </c>
       <c r="D637" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E637" s="8" t="s">
-        <v>1743</v>
+        <v>1724</v>
       </c>
       <c r="F637" s="2" t="s">
-        <v>1703</v>
+        <v>1657</v>
       </c>
       <c r="G637" s="8" t="s">
-        <v>1754</v>
+        <v>1818</v>
       </c>
       <c r="H637" s="8" t="s">
-        <v>1874</v>
+        <v>1868</v>
       </c>
       <c r="I637" s="2"/>
       <c r="J637" s="6">
@@ -25676,26 +25780,26 @@
       </c>
       <c r="B638" s="2"/>
       <c r="C638" s="3">
-        <v>40772</v>
+        <v>40750</v>
       </c>
       <c r="D638" s="2" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E638" s="8" t="s">
-        <v>1744</v>
+        <v>1725</v>
       </c>
       <c r="F638" s="2" t="s">
-        <v>1748</v>
+        <v>1737</v>
       </c>
       <c r="G638" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H638" s="8" t="s">
-        <v>1804</v>
+        <v>1869</v>
       </c>
       <c r="I638" s="2"/>
       <c r="J638" s="6">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="639" spans="1:10" s="1" customFormat="1">
@@ -25704,26 +25808,26 @@
       </c>
       <c r="B639" s="2"/>
       <c r="C639" s="3">
-        <v>40786</v>
+        <v>40757</v>
       </c>
       <c r="D639" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E639" s="8" t="s">
-        <v>1745</v>
+        <v>1738</v>
       </c>
       <c r="F639" s="2" t="s">
-        <v>1749</v>
+        <v>1747</v>
       </c>
       <c r="G639" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H639" s="8" t="s">
-        <v>1875</v>
+        <v>1870</v>
       </c>
       <c r="I639" s="2"/>
       <c r="J639" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="640" spans="1:10" s="1" customFormat="1">
@@ -25732,26 +25836,26 @@
       </c>
       <c r="B640" s="2"/>
       <c r="C640" s="3">
-        <v>40792</v>
+        <v>40758</v>
       </c>
       <c r="D640" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E640" s="8" t="s">
-        <v>977</v>
+        <v>1739</v>
       </c>
       <c r="F640" s="2" t="s">
-        <v>1750</v>
+        <v>15</v>
       </c>
       <c r="G640" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H640" s="8" t="s">
-        <v>1855</v>
+        <v>1871</v>
       </c>
       <c r="I640" s="2"/>
       <c r="J640" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="641" spans="1:10" s="1" customFormat="1">
@@ -25760,26 +25864,26 @@
       </c>
       <c r="B641" s="2"/>
       <c r="C641" s="3">
-        <v>40794</v>
+        <v>40759</v>
       </c>
       <c r="D641" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E641" s="8" t="s">
-        <v>977</v>
+        <v>1740</v>
       </c>
       <c r="F641" s="2" t="s">
-        <v>1751</v>
+        <v>506</v>
       </c>
       <c r="G641" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H641" s="8" t="s">
-        <v>1876</v>
+        <v>1872</v>
       </c>
       <c r="I641" s="2"/>
       <c r="J641" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="642" spans="1:10" s="1" customFormat="1">
@@ -25788,22 +25892,22 @@
       </c>
       <c r="B642" s="2"/>
       <c r="C642" s="3">
-        <v>40794</v>
+        <v>40760</v>
       </c>
       <c r="D642" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E642" s="8" t="s">
-        <v>1746</v>
+        <v>1741</v>
       </c>
       <c r="F642" s="2" t="s">
-        <v>1657</v>
+        <v>1747</v>
       </c>
       <c r="G642" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H642" s="8" t="s">
-        <v>1877</v>
+        <v>1800</v>
       </c>
       <c r="I642" s="2"/>
       <c r="J642" s="6">
@@ -25816,26 +25920,26 @@
       </c>
       <c r="B643" s="2"/>
       <c r="C643" s="3">
-        <v>40805</v>
+        <v>40760</v>
       </c>
       <c r="D643" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E643" s="8" t="s">
-        <v>1954</v>
+        <v>1742</v>
       </c>
       <c r="F643" s="2" t="s">
-        <v>494</v>
+        <v>49</v>
       </c>
       <c r="G643" s="8" t="s">
-        <v>1754</v>
+        <v>1756</v>
       </c>
       <c r="H643" s="8" t="s">
-        <v>1955</v>
+        <v>1873</v>
       </c>
       <c r="I643" s="2"/>
       <c r="J643" s="6">
-        <v>0.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="644" spans="1:10" s="1" customFormat="1">
@@ -25844,26 +25948,26 @@
       </c>
       <c r="B644" s="2"/>
       <c r="C644" s="3">
-        <v>40805</v>
+        <v>40772</v>
       </c>
       <c r="D644" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E644" s="8" t="s">
-        <v>1953</v>
+        <v>1743</v>
       </c>
       <c r="F644" s="2" t="s">
-        <v>1620</v>
+        <v>1703</v>
       </c>
       <c r="G644" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H644" s="8" t="s">
-        <v>1955</v>
+        <v>1874</v>
       </c>
       <c r="I644" s="2"/>
       <c r="J644" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="645" spans="1:10" s="1" customFormat="1">
@@ -25872,22 +25976,22 @@
       </c>
       <c r="B645" s="2"/>
       <c r="C645" s="3">
-        <v>40807</v>
+        <v>40772</v>
       </c>
       <c r="D645" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E645" s="8" t="s">
-        <v>1979</v>
+        <v>1744</v>
       </c>
       <c r="F645" s="2" t="s">
-        <v>1980</v>
+        <v>1748</v>
       </c>
       <c r="G645" s="8" t="s">
         <v>1754</v>
       </c>
       <c r="H645" s="8" t="s">
-        <v>1981</v>
+        <v>1804</v>
       </c>
       <c r="I645" s="2"/>
       <c r="J645" s="6">
@@ -25900,26 +26004,26 @@
       </c>
       <c r="B646" s="2"/>
       <c r="C646" s="3">
-        <v>40814</v>
+        <v>40786</v>
       </c>
       <c r="D646" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E646" s="8" t="s">
-        <v>2005</v>
+        <v>1745</v>
       </c>
       <c r="F646" s="2" t="s">
-        <v>506</v>
+        <v>1749</v>
       </c>
       <c r="G646" s="8" t="s">
-        <v>2006</v>
+        <v>1754</v>
       </c>
       <c r="H646" s="8" t="s">
-        <v>2007</v>
+        <v>1875</v>
       </c>
       <c r="I646" s="2"/>
       <c r="J646" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="647" spans="1:10" s="1" customFormat="1">
@@ -25928,26 +26032,26 @@
       </c>
       <c r="B647" s="2"/>
       <c r="C647" s="3">
-        <v>40816</v>
+        <v>40792</v>
       </c>
       <c r="D647" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E647" s="8" t="s">
-        <v>2008</v>
+        <v>977</v>
       </c>
       <c r="F647" s="2" t="s">
-        <v>49</v>
+        <v>1750</v>
       </c>
       <c r="G647" s="8" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="H647" s="8" t="s">
-        <v>2009</v>
+        <v>1855</v>
       </c>
       <c r="I647" s="2"/>
       <c r="J647" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="648" spans="1:10" s="1" customFormat="1">
@@ -25956,26 +26060,26 @@
       </c>
       <c r="B648" s="2"/>
       <c r="C648" s="3">
-        <v>40821</v>
+        <v>40794</v>
       </c>
       <c r="D648" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E648" s="8" t="s">
-        <v>2067</v>
+        <v>977</v>
       </c>
       <c r="F648" s="2" t="s">
-        <v>1092</v>
+        <v>1751</v>
       </c>
       <c r="G648" s="8" t="s">
-        <v>2070</v>
+        <v>1754</v>
       </c>
       <c r="H648" s="8" t="s">
-        <v>2071</v>
+        <v>1876</v>
       </c>
       <c r="I648" s="2"/>
       <c r="J648" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="649" spans="1:10" s="1" customFormat="1">
@@ -25984,26 +26088,26 @@
       </c>
       <c r="B649" s="2"/>
       <c r="C649" s="3">
-        <v>40822</v>
+        <v>40794</v>
       </c>
       <c r="D649" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E649" s="8" t="s">
-        <v>977</v>
+        <v>1746</v>
       </c>
       <c r="F649" s="2" t="s">
-        <v>2068</v>
+        <v>1657</v>
       </c>
       <c r="G649" s="8" t="s">
-        <v>2006</v>
+        <v>1754</v>
       </c>
       <c r="H649" s="8" t="s">
-        <v>2072</v>
+        <v>1877</v>
       </c>
       <c r="I649" s="2"/>
       <c r="J649" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="650" spans="1:10" s="1" customFormat="1">
@@ -26012,26 +26116,26 @@
       </c>
       <c r="B650" s="2"/>
       <c r="C650" s="3">
-        <v>40823</v>
+        <v>40805</v>
       </c>
       <c r="D650" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E650" s="8" t="s">
-        <v>977</v>
+        <v>1954</v>
       </c>
       <c r="F650" s="2" t="s">
-        <v>2069</v>
+        <v>494</v>
       </c>
       <c r="G650" s="8" t="s">
-        <v>2006</v>
+        <v>1754</v>
       </c>
       <c r="H650" s="8" t="s">
-        <v>2073</v>
+        <v>1955</v>
       </c>
       <c r="I650" s="2"/>
       <c r="J650" s="6">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="651" spans="1:10" s="1" customFormat="1">
@@ -26040,26 +26144,26 @@
       </c>
       <c r="B651" s="2"/>
       <c r="C651" s="3">
-        <v>40833</v>
+        <v>40805</v>
       </c>
       <c r="D651" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E651" s="8" t="s">
-        <v>2170</v>
+        <v>1953</v>
       </c>
       <c r="F651" s="2" t="s">
-        <v>1737</v>
+        <v>1620</v>
       </c>
       <c r="G651" s="8" t="s">
-        <v>2006</v>
+        <v>1754</v>
       </c>
       <c r="H651" s="8" t="s">
-        <v>2173</v>
+        <v>1955</v>
       </c>
       <c r="I651" s="2"/>
       <c r="J651" s="6">
-        <v>7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="652" spans="1:10" s="1" customFormat="1">
@@ -26068,26 +26172,26 @@
       </c>
       <c r="B652" s="2"/>
       <c r="C652" s="3">
-        <v>40840</v>
+        <v>40807</v>
       </c>
       <c r="D652" s="2" t="s">
-        <v>977</v>
+        <v>468</v>
       </c>
       <c r="E652" s="8" t="s">
-        <v>977</v>
+        <v>1979</v>
       </c>
       <c r="F652" s="2" t="s">
-        <v>2180</v>
+        <v>1980</v>
       </c>
       <c r="G652" s="8" t="s">
-        <v>2174</v>
+        <v>1754</v>
       </c>
       <c r="H652" s="8" t="s">
-        <v>2175</v>
+        <v>1981</v>
       </c>
       <c r="I652" s="2"/>
       <c r="J652" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="653" spans="1:10" s="1" customFormat="1">
@@ -26096,26 +26200,26 @@
       </c>
       <c r="B653" s="2"/>
       <c r="C653" s="3">
-        <v>40840</v>
+        <v>40814</v>
       </c>
       <c r="D653" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E653" s="8" t="s">
-        <v>2169</v>
+        <v>2005</v>
       </c>
       <c r="F653" s="2" t="s">
-        <v>1703</v>
+        <v>506</v>
       </c>
       <c r="G653" s="8" t="s">
         <v>2006</v>
       </c>
       <c r="H653" s="8" t="s">
-        <v>2176</v>
+        <v>2007</v>
       </c>
       <c r="I653" s="2"/>
       <c r="J653" s="6">
-        <v>8.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="654" spans="1:10" s="1" customFormat="1">
@@ -26124,26 +26228,26 @@
       </c>
       <c r="B654" s="2"/>
       <c r="C654" s="3">
-        <v>40844</v>
+        <v>40816</v>
       </c>
       <c r="D654" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E654" s="8" t="s">
-        <v>2168</v>
+        <v>2008</v>
       </c>
       <c r="F654" s="2" t="s">
         <v>49</v>
       </c>
       <c r="G654" s="8" t="s">
-        <v>2172</v>
+        <v>1756</v>
       </c>
       <c r="H654" s="8" t="s">
-        <v>2177</v>
+        <v>2009</v>
       </c>
       <c r="I654" s="2"/>
       <c r="J654" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="655" spans="1:10" s="1" customFormat="1">
@@ -26152,26 +26256,26 @@
       </c>
       <c r="B655" s="2"/>
       <c r="C655" s="3">
-        <v>40485</v>
+        <v>40821</v>
       </c>
       <c r="D655" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E655" s="8" t="s">
-        <v>2167</v>
+        <v>2067</v>
       </c>
       <c r="F655" s="2" t="s">
-        <v>2171</v>
+        <v>1092</v>
       </c>
       <c r="G655" s="8" t="s">
-        <v>2006</v>
+        <v>2070</v>
       </c>
       <c r="H655" s="8" t="s">
-        <v>2178</v>
+        <v>2071</v>
       </c>
       <c r="I655" s="2"/>
       <c r="J655" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="656" spans="1:10" s="1" customFormat="1">
@@ -26180,26 +26284,26 @@
       </c>
       <c r="B656" s="2"/>
       <c r="C656" s="3">
-        <v>40485</v>
+        <v>40822</v>
       </c>
       <c r="D656" s="2" t="s">
-        <v>468</v>
+        <v>977</v>
       </c>
       <c r="E656" s="8" t="s">
-        <v>2166</v>
+        <v>977</v>
       </c>
       <c r="F656" s="2" t="s">
-        <v>1703</v>
+        <v>2068</v>
       </c>
       <c r="G656" s="8" t="s">
         <v>2006</v>
       </c>
       <c r="H656" s="8" t="s">
-        <v>2179</v>
+        <v>2072</v>
       </c>
       <c r="I656" s="2"/>
       <c r="J656" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="657" spans="1:10" s="1" customFormat="1">
@@ -26208,7 +26312,7 @@
       </c>
       <c r="B657" s="2"/>
       <c r="C657" s="3">
-        <v>40857</v>
+        <v>40823</v>
       </c>
       <c r="D657" s="2" t="s">
         <v>977</v>
@@ -26217,142 +26321,366 @@
         <v>977</v>
       </c>
       <c r="F657" s="2" t="s">
-        <v>2212</v>
+        <v>2069</v>
       </c>
       <c r="G657" s="8" t="s">
         <v>2006</v>
       </c>
       <c r="H657" s="8" t="s">
-        <v>2213</v>
+        <v>2073</v>
       </c>
       <c r="I657" s="2"/>
       <c r="J657" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="658" spans="1:10" s="1" customFormat="1">
-      <c r="A658" s="2" t="s">
-        <v>1892</v>
+      <c r="A658" s="8" t="s">
+        <v>1617</v>
       </c>
       <c r="B658" s="2"/>
       <c r="C658" s="3">
-        <v>40611</v>
+        <v>40833</v>
       </c>
       <c r="D658" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="E658" s="2" t="s">
-        <v>1893</v>
+      <c r="E658" s="8" t="s">
+        <v>2170</v>
       </c>
       <c r="F658" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G658" s="2" t="s">
-        <v>1894</v>
-      </c>
-      <c r="H658" s="2" t="s">
-        <v>1895</v>
+        <v>1737</v>
+      </c>
+      <c r="G658" s="8" t="s">
+        <v>2006</v>
+      </c>
+      <c r="H658" s="8" t="s">
+        <v>2173</v>
       </c>
       <c r="I658" s="2"/>
       <c r="J658" s="6">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="659" spans="1:10" s="1" customFormat="1">
-      <c r="A659" s="2" t="s">
-        <v>1896</v>
+      <c r="A659" s="8" t="s">
+        <v>1617</v>
       </c>
       <c r="B659" s="2"/>
       <c r="C659" s="3">
-        <v>40338</v>
+        <v>40840</v>
       </c>
       <c r="D659" s="2" t="s">
-        <v>913</v>
-      </c>
-      <c r="E659" s="2"/>
-      <c r="F659" s="2"/>
-      <c r="G659" s="2" t="s">
-        <v>1897</v>
-      </c>
-      <c r="H659" s="2" t="s">
-        <v>1898</v>
+        <v>977</v>
+      </c>
+      <c r="E659" s="8" t="s">
+        <v>977</v>
+      </c>
+      <c r="F659" s="2" t="s">
+        <v>2180</v>
+      </c>
+      <c r="G659" s="8" t="s">
+        <v>2174</v>
+      </c>
+      <c r="H659" s="8" t="s">
+        <v>2175</v>
       </c>
       <c r="I659" s="2"/>
-      <c r="J659" s="6"/>
-    </row>
-    <row r="660" spans="1:10">
-      <c r="A660" s="2" t="s">
-        <v>1896</v>
+      <c r="J659" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="660" spans="1:10" s="1" customFormat="1">
+      <c r="A660" s="8" t="s">
+        <v>1617</v>
       </c>
       <c r="B660" s="2"/>
       <c r="C660" s="3">
-        <v>40350</v>
+        <v>40840</v>
       </c>
       <c r="D660" s="2" t="s">
-        <v>913</v>
-      </c>
-      <c r="E660" s="2"/>
-      <c r="F660" s="2"/>
-      <c r="G660" s="2" t="s">
-        <v>1899</v>
-      </c>
-      <c r="H660" s="2" t="s">
-        <v>1900</v>
-      </c>
-      <c r="I660" s="2" t="s">
-        <v>1901</v>
-      </c>
-      <c r="J660" s="6"/>
-    </row>
-    <row r="661" spans="1:10">
-      <c r="A661" s="2" t="s">
-        <v>1896</v>
+        <v>468</v>
+      </c>
+      <c r="E660" s="8" t="s">
+        <v>2169</v>
+      </c>
+      <c r="F660" s="2" t="s">
+        <v>1703</v>
+      </c>
+      <c r="G660" s="8" t="s">
+        <v>2006</v>
+      </c>
+      <c r="H660" s="8" t="s">
+        <v>2176</v>
+      </c>
+      <c r="I660" s="2"/>
+      <c r="J660" s="6">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="661" spans="1:10" s="1" customFormat="1">
+      <c r="A661" s="8" t="s">
+        <v>1617</v>
       </c>
       <c r="B661" s="2"/>
       <c r="C661" s="3">
-        <v>40378</v>
+        <v>40844</v>
       </c>
       <c r="D661" s="2" t="s">
-        <v>913</v>
-      </c>
-      <c r="E661" s="2"/>
-      <c r="F661" s="2"/>
-      <c r="G661" s="2" t="s">
-        <v>1902</v>
-      </c>
-      <c r="H661" s="2" t="s">
-        <v>1904</v>
-      </c>
-      <c r="I661" s="2" t="s">
-        <v>1903</v>
-      </c>
-      <c r="J661" s="6"/>
-    </row>
-    <row r="662" spans="1:10">
+        <v>468</v>
+      </c>
+      <c r="E661" s="8" t="s">
+        <v>2168</v>
+      </c>
+      <c r="F661" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G661" s="8" t="s">
+        <v>2172</v>
+      </c>
+      <c r="H661" s="8" t="s">
+        <v>2177</v>
+      </c>
+      <c r="I661" s="2"/>
+      <c r="J661" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="662" spans="1:10" s="1" customFormat="1">
       <c r="A662" s="8" t="s">
-        <v>1905</v>
+        <v>1617</v>
       </c>
       <c r="B662" s="2"/>
       <c r="C662" s="3">
-        <v>40795</v>
+        <v>40485</v>
       </c>
       <c r="D662" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="E662" s="2" t="s">
-        <v>1906</v>
+      <c r="E662" s="8" t="s">
+        <v>2167</v>
       </c>
       <c r="F662" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G662" s="2" t="s">
-        <v>1907</v>
-      </c>
-      <c r="H662" s="2" t="s">
-        <v>1908</v>
+        <v>2171</v>
+      </c>
+      <c r="G662" s="8" t="s">
+        <v>2006</v>
+      </c>
+      <c r="H662" s="8" t="s">
+        <v>2178</v>
       </c>
       <c r="I662" s="2"/>
       <c r="J662" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="663" spans="1:10" s="1" customFormat="1">
+      <c r="A663" s="8" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B663" s="2"/>
+      <c r="C663" s="3">
+        <v>40485</v>
+      </c>
+      <c r="D663" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E663" s="8" t="s">
+        <v>2166</v>
+      </c>
+      <c r="F663" s="2" t="s">
+        <v>1703</v>
+      </c>
+      <c r="G663" s="8" t="s">
+        <v>2006</v>
+      </c>
+      <c r="H663" s="8" t="s">
+        <v>2179</v>
+      </c>
+      <c r="I663" s="2"/>
+      <c r="J663" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="664" spans="1:10" s="1" customFormat="1">
+      <c r="A664" s="8" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B664" s="2"/>
+      <c r="C664" s="3">
+        <v>40857</v>
+      </c>
+      <c r="D664" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="E664" s="8" t="s">
+        <v>977</v>
+      </c>
+      <c r="F664" s="2" t="s">
+        <v>2212</v>
+      </c>
+      <c r="G664" s="8" t="s">
+        <v>2006</v>
+      </c>
+      <c r="H664" s="8" t="s">
+        <v>2213</v>
+      </c>
+      <c r="I664" s="2"/>
+      <c r="J664" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="665" spans="1:10" s="1" customFormat="1">
+      <c r="A665" s="8" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B665" s="2"/>
+      <c r="C665" s="3">
+        <v>40875</v>
+      </c>
+      <c r="D665" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E665" s="8" t="s">
+        <v>2284</v>
+      </c>
+      <c r="F665" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G665" s="8" t="s">
+        <v>2285</v>
+      </c>
+      <c r="H665" s="8" t="s">
+        <v>2286</v>
+      </c>
+      <c r="I665" s="2"/>
+      <c r="J665" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="666" spans="1:10" s="1" customFormat="1">
+      <c r="A666" s="2" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B666" s="2"/>
+      <c r="C666" s="3">
+        <v>40611</v>
+      </c>
+      <c r="D666" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="E666" s="2" t="s">
+        <v>1893</v>
+      </c>
+      <c r="F666" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G666" s="2" t="s">
+        <v>1894</v>
+      </c>
+      <c r="H666" s="2" t="s">
+        <v>1895</v>
+      </c>
+      <c r="I666" s="2"/>
+      <c r="J666" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="667" spans="1:10" s="1" customFormat="1">
+      <c r="A667" s="2" t="s">
+        <v>1896</v>
+      </c>
+      <c r="B667" s="2"/>
+      <c r="C667" s="3">
+        <v>40338</v>
+      </c>
+      <c r="D667" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="E667" s="2"/>
+      <c r="F667" s="2"/>
+      <c r="G667" s="2" t="s">
+        <v>1897</v>
+      </c>
+      <c r="H667" s="2" t="s">
+        <v>1898</v>
+      </c>
+      <c r="I667" s="2"/>
+      <c r="J667" s="6"/>
+    </row>
+    <row r="668" spans="1:10">
+      <c r="A668" s="2" t="s">
+        <v>1896</v>
+      </c>
+      <c r="B668" s="2"/>
+      <c r="C668" s="3">
+        <v>40350</v>
+      </c>
+      <c r="D668" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="E668" s="2"/>
+      <c r="F668" s="2"/>
+      <c r="G668" s="2" t="s">
+        <v>1899</v>
+      </c>
+      <c r="H668" s="2" t="s">
+        <v>1900</v>
+      </c>
+      <c r="I668" s="2" t="s">
+        <v>1901</v>
+      </c>
+      <c r="J668" s="6"/>
+    </row>
+    <row r="669" spans="1:10">
+      <c r="A669" s="2" t="s">
+        <v>1896</v>
+      </c>
+      <c r="B669" s="2"/>
+      <c r="C669" s="3">
+        <v>40378</v>
+      </c>
+      <c r="D669" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="E669" s="2"/>
+      <c r="F669" s="2"/>
+      <c r="G669" s="2" t="s">
+        <v>1902</v>
+      </c>
+      <c r="H669" s="2" t="s">
+        <v>1904</v>
+      </c>
+      <c r="I669" s="2" t="s">
+        <v>1903</v>
+      </c>
+      <c r="J669" s="6"/>
+    </row>
+    <row r="670" spans="1:10">
+      <c r="A670" s="8" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B670" s="2"/>
+      <c r="C670" s="3">
+        <v>40795</v>
+      </c>
+      <c r="D670" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E670" s="2" t="s">
+        <v>1906</v>
+      </c>
+      <c r="F670" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G670" s="2" t="s">
+        <v>1907</v>
+      </c>
+      <c r="H670" s="2" t="s">
+        <v>1908</v>
+      </c>
+      <c r="I670" s="2"/>
+      <c r="J670" s="6">
         <v>5</v>
       </c>
     </row>

</xml_diff>